<commit_message>
Update model, data, and job tracking files
Retrained the AI model and vectorizer, updated jobs.xlsx, expanded labels.json with new job entries, and added corresponding entries to seen_jobs_muisz.txt and seen_jobs_schonherz.txt for improved job tracking and classification.
</commit_message>
<xml_diff>
--- a/data/jobs.xlsx
+++ b/data/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,36 +631,36 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer Intern</t>
+          <t>AI-assisted developer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40713-machine-learning-engineer-intern</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40704-ai-assisted-developer</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📍Our Partner provides a platform that supports requirements engineering, development, and testing in both Agile and V-model processes. It enhances productivity and quality by enabling knowledge reuse, semantic search, and the detection of duplicates, similarities, and inconsistencies, as well as offering contextual and domain-specific authoring support. The platform integrates seamlessly with a wide range of software engineering tools, ensuring compatibility and ease of use, and can be deployed on-premise or as a SaaS solution. 🤖 The company is looking for a highly motivated Machine Learning Intern to join its dynamic team. In this role, the intern will support the AI team in their daily operations. Responsibilities: 🧠 Assist in the design, development, and deployment of machine learning models 📊 Work with large datasets, including data preprocessing, feature engineering, and analysis 🤝 Collaborate with the team to improve the accuracy and performance of machine learning models ⚙️ Maintain automated pipelines for model training, testing, and evaluation Requirements: 🎓 Ongoing Bachelor’s or Master’s studies (a must) 📘 Preferred fields: Computer Engineering, Software Engineering, Bioinformatics, Electrical Engineering, or potentially Finance 🤖 Strong interest and/or experience in: • LLM fine-tuning • Retrieval-Augmented Generation (RAG) • Machine Learning / Deep Learning • NLP / GenAI • Computer Vision / Object Detection 🐍 Practical experience with Python and PyTorch 🗣️ Language skills: 🇨🇳 Fluent Chinese (native or advanced) 🇬🇧 English at B2 level or higher ❗ Hungarian is not required 🤝 Ability to work collaboratively across teams 📌 Capable of managing multiple priorities effectively 🌟 Enjoys working in a highly skilled, competitive team with flat hierarchies 🎁 What our Partner offers: 🌍 Flexible working location and flexible working hours 🤝 Strong team spirit, with a mentor/buddy program to support your onboarding 🏆 Access to world-class clients and a cutting-edge product shaping the next industrial revolution 💰 Competitive remuneration 🎉 Regular offsite team-building events 🏢 Modern office located at Deák Ferenc tér 🕘 Working arrangement: flexible, primarily remote work, with approximately one day per month required in the office ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Send us your english CV with a photo to the hr@schonherz.hu e-mail adress! * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 656,785 per month.</t>
+          <t>💼 Our partner is a dynamic and innovative Irish-based company offering cloud-based streaming and virtual cinema experiences. They build digital platforms for film enthusiasts, event organizers, and educational institutions. 👉 You can join a youthful, creative team working on exciting projects at the intersection of technology and entertainment. Task: 🤖 Developing software using AI tools and utilising existing web services Expectations: ⏹️ Ongoing higher education studies ⏹️ Experience with AI coding tools ⏹️ NodeJS, Javascript knowledge ⏹️ Client-side programming ⏹️ Using backend web services (REST) ⏹️ UI design ⏹️ Cover letter in English ⏹️ Examples of previous work in CV, which can be viewed online ⏹️ Advanced written and spoken English skills ⏹️ Good communication skills ⏹️ Ability to work unsupervised ⏰ Working hours: Core hours on working days of 10:00-16:00 or other hours as agreed, the usual is 3 days in the office and 2 days work from home but only after a trial period if we know the employee can work unsupervised ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Fill in a CV on Schönherz.hu * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 656,785 per month.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>English and Chinese (fluent)</t>
+          <t>English (Advanced)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Home office</t>
+          <t>Budapest, District III + Home Office</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Gross 3000 Ft/hour*</t>
+          <t>Gross 3500 Ft/hour*</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -675,32 +675,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AI-assisted developer</t>
+          <t>Programozó munkatárs</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40704-ai-assisted-developer</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40699-programozo-munkatars</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>💼 Our partner is a dynamic and innovative Irish-based company offering cloud-based streaming and virtual cinema experiences. They build digital platforms for film enthusiasts, event organizers, and educational institutions. 👉 You can join a youthful, creative team working on exciting projects at the intersection of technology and entertainment. Task: 🤖 Developing software using AI tools and utilising existing web services Expectations: ⏹️ Ongoing higher education studies ⏹️ Experience with AI coding tools ⏹️ NodeJS, Javascript knowledge ⏹️ Client-side programming ⏹️ Using backend web services (REST) ⏹️ UI design ⏹️ Cover letter in English ⏹️ Examples of previous work in CV, which can be viewed online ⏹️ Advanced written and spoken English skills ⏹️ Good communication skills ⏹️ Ability to work unsupervised ⏰ Working hours: Core hours on working days of 10:00-16:00 or other hours as agreed, the usual is 3 days in the office and 2 days work from home but only after a trial period if we know the employee can work unsupervised ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Fill in a CV on Schönherz.hu * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 656,785 per month.</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>English (Advanced)</t>
-        </is>
-      </c>
+          <t>✨ Partnerünk 1999-ben alakult, és azóta is megbízható szereplője a nyomdai és reklámdekorációs piacnak. Digitális nyomdai termékek tervezésében, gyártásában, valamint helyszíni kivitelezésében nyújt segítséget ügyfeleinek, rövid határidővel, gyors és pontos munkavégzéssel. A különböző szakterületeken dolgozó munkatársai sokéves tapasztalattal rendelkeznek, és elkötelezettek abban, hogy a megrendelők reklámdekorációs elképzeléseit maradéktalanul megvalósítsák. Feladatok: 🦜 Webfejlesztési feladatok ellátása 🦜 Dokumentációk elkészítése 🦜 A cél: nem sablon, hanem egyedi funkcionális bővítmények fejlesztése Elvárások: 🔘 Folyamatban lévő felsőfokú informatikai tanulmányok 🔘 PHP (vanilla) középhaladó szintű ismerete 🔘 Tiszta kódszerkezet és funkcionális szemlélet 🔘 OOP alapok: osztályok, property-k, konstruktor, metódusok ismerete 🔘 Adatkezelés: tömbök, stringek, json_encode/decode, fájlműveletek 🔘 Képesség curl, file_get_contents külső tartalmak kezelésére 🔘 Alap szintű HTML DOM feldolgozás: DOMDocument, DOMXPath JavaScript (vanilla, modern szemlélettel) 🔘 DOM-manipuláció, eseménykezelés, querySelector, stb. 🔘 Form-kezelés (valós idejű validáció, AJAX/Fetch küldés) 🔘 Modularitás (külön JS fájlok, függvények, struktúra) 🔘 Interaktív UI komponensek Bootstrap 5 segítségével -Frontend 🔘 Bootstrap 5 rutinszintű használata (grid, modal, form, alert) 🔘 Reszponzív nézetek, breakpoints, Flexbox/Grid kombinálása 🔘 Letisztult, minimális, de igényes UI kivitelezés -WordPress (strukturált pluginfejlesztés) 🔘 Shortcode pluginok készítése nulláról (függvények, HTML, JS) 🔘 Elementor-kompatibilitás szem előtt tartása (output, elrendezés) 🔘 add_shortcode, wp_enqueue_script, wp_register_style rutinszintű ismerete 🔘 Rendszerben gondolkodik: nem csak megold egy feladatot, hanem illeszti a meglévő struktúrához 🔘 Olvasható, kommentelt, jól tagolt kódot ír 🔘 Tisztában van a fájlstruktúrák szerepével (pl. application, core, config, public, stb.) 🔘 Nyitott az iteratív fejlesztésre: első verzió › visszajelzés › finomítás 🔘 Képes önállóan hibát keresni (console, log, var_dump, try-catch, stb.) Előnyök: 🔻 JSON ↔ CSV, slug generátor, meta tag parser típusú eszközlogikák 🔻 SEO-barát struktúrák: pl. URL-séma, output tisztítás, canonical linkek Amit Partnerünk kínál: ⏹️ Irodai munkakörnyezet 🧙‍♂️ Senior kolléga mellett tanulhatsz 🏡 Home Office lehetőség ⏰ Munkaidő: Általános irodai munkarend, hétköznaponta 08:00-17:00 között rugalmasan, a Partner osztja be a feladatokat ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 656 785 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Budapest, District III + Home Office</t>
+          <t>Budaörs + Home office</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Gross 3500 Ft/hour*</t>
+          <t>Br. 2005-2300 Ft/óra*</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -719,32 +715,36 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Programozó munkatárs</t>
+          <t>Symfony fejlesztő, Full-Stack lehetősséggel</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40699-programozo-munkatars</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40635-symfony-fejleszto-full-stack-lehetosseggel</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>✨ Partnerünk 1999-ben alakult, és azóta is megbízható szereplője a nyomdai és reklámdekorációs piacnak. Digitális nyomdai termékek tervezésében, gyártásában, valamint helyszíni kivitelezésében nyújt segítséget ügyfeleinek, rövid határidővel, gyors és pontos munkavégzéssel. A különböző szakterületeken dolgozó munkatársai sokéves tapasztalattal rendelkeznek, és elkötelezettek abban, hogy a megrendelők reklámdekorációs elképzeléseit maradéktalanul megvalósítsák. Feladatok: 🦜 Webfejlesztési feladatok ellátása 🦜 Dokumentációk elkészítése 🦜 A cél: nem sablon, hanem egyedi funkcionális bővítmények fejlesztése Elvárások: 🔘 Folyamatban lévő felsőfokú informatikai tanulmányok 🔘 PHP (vanilla) középhaladó szintű ismerete 🔘 Tiszta kódszerkezet és funkcionális szemlélet 🔘 OOP alapok: osztályok, property-k, konstruktor, metódusok ismerete 🔘 Adatkezelés: tömbök, stringek, json_encode/decode, fájlműveletek 🔘 Képesség curl, file_get_contents külső tartalmak kezelésére 🔘 Alap szintű HTML DOM feldolgozás: DOMDocument, DOMXPath JavaScript (vanilla, modern szemlélettel) 🔘 DOM-manipuláció, eseménykezelés, querySelector, stb. 🔘 Form-kezelés (valós idejű validáció, AJAX/Fetch küldés) 🔘 Modularitás (külön JS fájlok, függvények, struktúra) 🔘 Interaktív UI komponensek Bootstrap 5 segítségével -Frontend 🔘 Bootstrap 5 rutinszintű használata (grid, modal, form, alert) 🔘 Reszponzív nézetek, breakpoints, Flexbox/Grid kombinálása 🔘 Letisztult, minimális, de igényes UI kivitelezés -WordPress (strukturált pluginfejlesztés) 🔘 Shortcode pluginok készítése nulláról (függvények, HTML, JS) 🔘 Elementor-kompatibilitás szem előtt tartása (output, elrendezés) 🔘 add_shortcode, wp_enqueue_script, wp_register_style rutinszintű ismerete 🔘 Rendszerben gondolkodik: nem csak megold egy feladatot, hanem illeszti a meglévő struktúrához 🔘 Olvasható, kommentelt, jól tagolt kódot ír 🔘 Tisztában van a fájlstruktúrák szerepével (pl. application, core, config, public, stb.) 🔘 Nyitott az iteratív fejlesztésre: első verzió › visszajelzés › finomítás 🔘 Képes önállóan hibát keresni (console, log, var_dump, try-catch, stb.) Előnyök: 🔻 JSON ↔ CSV, slug generátor, meta tag parser típusú eszközlogikák 🔻 SEO-barát struktúrák: pl. URL-séma, output tisztítás, canonical linkek Amit Partnerünk kínál: ⏹️ Irodai munkakörnyezet 🧙‍♂️ Senior kolléga mellett tanulhatsz 🏡 Home Office lehetőség ⏰ Munkaidő: Általános irodai munkarend, hétköznaponta 08:00-17:00 között rugalmasan, a Partner osztja be a feladatokat ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 656 785 Ft havonta.</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>☁️ A Partnerünk saját fejlesztésű felhőalapú vállalatirányítási rendszert kínál (ERP – Enterprise Resource Planning), amely képes integrálni a vállalat különböző folyamatait — mint például értékesítés, beszerzés, termelés, pénzügy, raktározás, ügyfélszolgálat stb. Szolgáltatásuk célja, hogy közép- és kisvállalatok számára hatékonyabbá tegyék az üzleti működést, csökkentsék a költségeket és növeljék a termelékenységet anélkül, hogy saját IT-infrastruktúrába kellene beruházniuk. Feladataid: 🔘 Meglévő modulok továbbfejlesztése 🔘 Új funkciók és modulok fejlesztése 🔘 Kisebb, önálló feladatok megoldása 🔘 Backend fejlesztési feladatok ellátása Symfony keretrendszer használatával Elvárások: 🌵 Folyamatban lévő felsőfokú tanulmányok 🌵 Alapvető PHP -Symfony ismeretek fontosak, de ha már dolgoztál Laravel keretrendszerrel annak is örülünk 🌵 Igényes, átgondolt munkavégzés 🌵 Nyitottság a tanulásra és a csapatmunkára 🌵 Érdeklődés az API-k és felhőalapú megoldások iránt 🌵 AI-eszközök használata a munkád támogatására - az AI használata a munkád során nem tiltott, sőt örülnek, ha segédeszközként tekintesz rá, de azért a saját tudásodra is támaszkodj 🌵 Angol nyelvtudás középfokon, írásban Amit Partnerünk kínál: 📐 Hosszútávra terveznek Veled 📖 Lehetőséget biztosítanak Udemy kurzusok elsajátítására 📚 A szakdolgozatod írása során szívesen vállalnak konzulensi feladatot 🟡 Dolgozhatsz Full-Stack fejlesztőként is, amennyiben az előnyöknél említett Frontend keretrendszereket is jól ismered ⏳ Lehetőség hosszú távú együttműködésre a tanulmányaid befejezése után is ⏰ Munkaidő: Kötetlen munkarend, de heti 2 személyes alkalom van, amikor egy köztes helyen vagy coworking irodában összeül a csapat és személyesen egyeztetnek 🔻 Adott esetben tudják úgy szervezni, hogy ne ütközzön az óráiddal, de ezeken a megbeszéléseken fontos, hogy megjelenj ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 656 785 Ft havonta!</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Angol (Középfok)</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Budaörs + Home office</t>
+          <t>Home Office</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Br. 2005-2300 Ft/óra*</t>
+          <t>Br. 2500-3500 Ft/óra*</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -754,35 +754,39 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>schonherz</t>
+          <t>muisz</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Fejlesztőmérnök</t>
+          <t>IT gyakornok</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40636-fejlesztomernok</t>
+          <t>https://muisz.hu/diakmunkaink/kepzes-fejlesztesi-gyakornok-budapest-10-ker--28184</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>📐 Partnercégünk a csomagolástechnikában alkalmazott, nyomaték- és erőmérő műszerek gyártásának nemzetközileg elismert, exportorientált szereplője. Feladatok: 🎁 Egyedi nyomaték- és erőmérő rendszerek fejlesztése 🎁 Elektronikai és mechanikai komponensek integrálása 🎁 Gépek összeszerelése, tesztelése, kalibárlása 🎁 Szoftverfejlesztés és tesztelés (C++, PLC ladder logic) 🎁 (Mechatronikus esetén) 3D modellezés SolidWorks-ben Elvárások: ✅ Folyamatban lévő felsőfokú tanulmányok BME, esetleg Óbudai Egyetem, vagy hasonló egyetemeken ✅ Magas szintű C++ programozási ismeret ✅ PLC ladder logic ismerete ✅ Angol nyelvtudás legalább középszinten (műszaki dokumentáció szintjén) ✅ 3D modellezés tapasztalat SolidWorks-ben ✅ Precizitás, önállóság ✅ Jó problémamegoldó szemlélet Amit Partnerünk kínál: 🧩 Hosszú távú, stabil mérnöki munka kis csapatban, angol nyelvi környezetben 📍 Teljes vagy részmunkaidős foglalkoztatás 💎 Valódi termékfejlesztési tapasztalat, nem „összeszerelés” 💸 Versenyképes jövedelem ⏳ Rugalmas munkaidő 🎲 Szakmai fejlődési lehetőség 🖥️ Színvonalas munkakörnyezet ⏰ Munkaidő: általános irodai munkarend (kb. 08:00-17:00 között), Partner osztja be a diákkal rugalmasan egyeztetve ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 656 785 Ft havonta!</t>
+          <t>IT gyakornok A Continental korábbi Automotive üzleti szektora a 2025 szeptemberi függetlenné válását követően AUMOVIO néven folytatja tevékenységét. A technológiai és elektronikai vállalat széles portfóliót kínál, amely biztonságossá, élvezetessé, összekapcsolttá és autonómmá teszi a mobilitást. Termékkínálatába többek között szenzoros megoldások, kijelzők, fék- és kényelmi rendszerek tartoznak. Emellett kiterjedt szakértelemmel rendelkezik a szoftverek, architektúra-platformok és a szoftveralapú járművekhez kapcsolódó vezetéstámogató rendszerek terén. A 2024-es pénzügyi évben az AUMOVIO-hoz tartozó üzleti területek 19,6 milliárd euró árbevételt értek el. A vállalat központja Frankfurtban, Németországban található, és világszerte több mint 100 telephelyen mintegy 87 000 munkatársat foglalkoztat. Feladatok Amiben a Te segítségedre számítunk: •	Irodai és gyártási gépek telepítésében •	Céges mobil telepítésében és teljes körű előkészítésében •	Kezdő szinten NMR használatában •	Ticketek kezelésében •	Felhasználói támogatásban Elvárások Te vagy az ideális jelölt, ha: •	Jelenleg felsőfokú tanulmányokat folytatsz – ideálisan informatikai területen •	Nappali tagozatos, aktív hallgatói jogviszonnyal rendelkezel még legalább egy évig •	Felhasználói szinten kezeled a MS Office-t •	Legalább heti 20-25 órát tudsz vállalni •	Középfokú angol nyelvtudással rendelkezel •	Precízen és pontosan végzed el a rád bízott feladatokat •	 Rugalmas hozzáállással rendelkezel Egyéb Amiért megéri nálunk dolgozni: •	a legkorszerűbb elektronikai gyártási technológiák, a legkiválóbb szakemberek •	versenyképes jövedelem •	tapasztalatot szerezhetsz egy gyártó cég folyamataiban, melyet szakdolgozatod írásához is felhasználhatsz •	dinamikus, fiatalos vállalati kultúrában, multinacionális környezetben dolgozhatsz •	hosszú távon számítunk Rád</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Angol (Középfok)</t>
+          <t>magyar, angol</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Budapest, XXII. kerület</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
+          <t>Budapest 10. ker.</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2709 Ft/óra</t>
+        </is>
+      </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
@@ -794,37 +798,37 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>schonherz</t>
+          <t>muisz</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Symfony fejlesztő, Full-Stack lehetősséggel</t>
+          <t>Student for IT Support &amp; Virtual Integration Tester</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40635-symfony-fejleszto-full-stack-lehetosseggel</t>
+          <t>https://muisz.hu/diakmunkaink/IT-support-trainee%20-xi-kerulet--28247</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>☁️ A Partnerünk saját fejlesztésű felhőalapú vállalatirányítási rendszert kínál (ERP – Enterprise Resource Planning), amely képes integrálni a vállalat különböző folyamatait — mint például értékesítés, beszerzés, termelés, pénzügy, raktározás, ügyfélszolgálat stb. Szolgáltatásuk célja, hogy közép- és kisvállalatok számára hatékonyabbá tegyék az üzleti működést, csökkentsék a költségeket és növeljék a termelékenységet anélkül, hogy saját IT-infrastruktúrába kellene beruházniuk. Feladataid: 🔘 Meglévő modulok továbbfejlesztése 🔘 Új funkciók és modulok fejlesztése 🔘 Kisebb, önálló feladatok megoldása 🔘 Backend fejlesztési feladatok ellátása Symfony keretrendszer használatával Elvárások: 🌵 Folyamatban lévő felsőfokú tanulmányok 🌵 Alapvető PHP -Symfony ismeretek fontosak, de ha már dolgoztál Laravel keretrendszerrel annak is örülünk 🌵 Igényes, átgondolt munkavégzés 🌵 Nyitottság a tanulásra és a csapatmunkára 🌵 Érdeklődés az API-k és felhőalapú megoldások iránt 🌵 AI-eszközök használata a munkád támogatására - az AI használata a munkád során nem tiltott, sőt örülnek, ha segédeszközként tekintesz rá, de azért a saját tudásodra is támaszkodj 🌵 Angol nyelvtudás középfokon, írásban Amit Partnerünk kínál: 📐 Hosszútávra terveznek Veled 📖 Lehetőséget biztosítanak Udemy kurzusok elsajátítására 📚 A szakdolgozatod írása során szívesen vállalnak konzulensi feladatot 🟡 Dolgozhatsz Full-Stack fejlesztőként is, amennyiben az előnyöknél említett Frontend keretrendszereket is jól ismered ⏳ Lehetőség hosszú távú együttműködésre a tanulmányaid befejezése után is ⏰ Munkaidő: Kötetlen munkarend, de heti 2 személyes alkalom van, amikor egy köztes helyen vagy coworking irodában összeül a csapat és személyesen egyeztetnek 🔻 Adott esetben tudják úgy szervezni, hogy ne ütközzön az óráiddal, de ezeken a megbeszéléseken fontos, hogy megjelenj ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 656 785 Ft havonta!</t>
+          <t>Student for IT Support &amp; Virtual Integration Tester Today the community of around 1800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. Join a dynamic and innovative team that is shaping the future of surgical imaging! We are developing a cutting-edge framework that enables C-arms to seamlessly integrate and run surgical software applications without compromising core functionality. You’ll work in a colocated development team, while collaborating with an international business network.  You will have the opportunity to learn and contribute to the development of a market-leading product that is already making a real impact in healthcare. If you love technology, problem-solving, and making an impact in healthcare, this is your chance! Feladatok •	Assist with system testing and installations. •	Work with Windows environments, including PowerShell scripting and basic network configuration. •	Support the setup and troubleshooting of our virtual integration testing environment. •	Contribute to improvements and maintenance of virtualization solutions (preferably Hyper-V, or similar technologies). •	Collaborate on tasks involving C#/.NET development for integration and automation purposes. Elvárások •	Ongoing university studies in a realated filed. •	Solid understanding of Windows OS and PowerShell. •	Basic knowledge of networking concepts. •	Experience with virtualization platforms (Hyper-V or similar). •	Familiarity with C#/.NET is a strong advantage. •	Problem-solving mindset and willingness to learn new technologies. Egyéb What we offer: •	Hybrid work model: 3 days/week home office opportunity (on average) •	Flexible working hours •	A young, dynamic, supporting team with mentor •	Attractive working environment and secure workplace •	Opportunity for international work experience •	Training possibilities: Language, soft-skill and technical trainings, corporate programs, meetups •	Various career opportunities •	Loyalty programs (Siemens Share Matching Program and Company loan opportunity) •	You can join several communities: sport, CSR, Go green, ToastMasters, etc. •	Family Friendly Workplace</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Angol (Középfok)</t>
+          <t>magyar, angol</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Home Office</t>
+          <t>Budapest 11. ker.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Br. 2500-3500 Ft/óra*</t>
+          <t>2200-2800 Ft/óra</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -843,17 +847,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IT gyakornok</t>
+          <t>Test framework developer trainee</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/kepzes-fejlesztesi-gyakornok-budapest-10-ker--28184</t>
+          <t>https://muisz.hu/diakmunkaink/Test-framework-developer-trainee%20-xi-kerulet--28240</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>IT gyakornok A Continental korábbi Automotive üzleti szektora a 2025 szeptemberi függetlenné válását követően AUMOVIO néven folytatja tevékenységét. A technológiai és elektronikai vállalat széles portfóliót kínál, amely biztonságossá, élvezetessé, összekapcsolttá és autonómmá teszi a mobilitást. Termékkínálatába többek között szenzoros megoldások, kijelzők, fék- és kényelmi rendszerek tartoznak. Emellett kiterjedt szakértelemmel rendelkezik a szoftverek, architektúra-platformok és a szoftveralapú járművekhez kapcsolódó vezetéstámogató rendszerek terén. A 2024-es pénzügyi évben az AUMOVIO-hoz tartozó üzleti területek 19,6 milliárd euró árbevételt értek el. A vállalat központja Frankfurtban, Németországban található, és világszerte több mint 100 telephelyen mintegy 87 000 munkatársat foglalkoztat. Feladatok Amiben a Te segítségedre számítunk: •	Irodai és gyártási gépek telepítésében •	Céges mobil telepítésében és teljes körű előkészítésében •	Kezdő szinten NMR használatában •	Ticketek kezelésében •	Felhasználói támogatásban Elvárások Te vagy az ideális jelölt, ha: •	Jelenleg felsőfokú tanulmányokat folytatsz – ideálisan informatikai területen •	Nappali tagozatos, aktív hallgatói jogviszonnyal rendelkezel még legalább egy évig •	Felhasználói szinten kezeled a MS Office-t •	Legalább heti 20-25 órát tudsz vállalni •	Középfokú angol nyelvtudással rendelkezel •	Precízen és pontosan végzed el a rád bízott feladatokat •	 Rugalmas hozzáállással rendelkezel Egyéb Amiért megéri nálunk dolgozni: •	a legkorszerűbb elektronikai gyártási technológiák, a legkiválóbb szakemberek •	versenyképes jövedelem •	tapasztalatot szerezhetsz egy gyártó cég folyamataiban, melyet szakdolgozatod írásához is felhasználhatsz •	dinamikus, fiatalos vállalati kultúrában, multinacionális környezetben dolgozhatsz •	hosszú távon számítunk Rád</t>
+          <t>Test framework developer trainee “Today the community of around 1,800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems, and you can even find them/us in electric cars. There are hardly any industrial areas where the programs our colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members 30 years ago. As of today, our headcount has nearly reached 1,800 employees and we are expanding – join us, be part of our team!” We are looking for a new colleague who will join our office in Budapest: Feladatok •	Implement and write tests for Angular web applications •	Work in a team and actively communicate with members •	Be able to work independently Elvárások •	Ongoing higher education studies (software engineering or similar) •	Angular or React experience •	Communication level English •	Have strong understanding of programming paradigms •	Good communication and problem-solving skills, systems thinking Egyéb Advantages: •	Software development experience in Web applications •	Experience in UI automation •	DevOps experience What we offer: •	A young, dynamic, supporting team with mentor(s) •	Thesis topic and writing opportunity with an in-house consultant •	Home Office opportunity, flexible working hours •	Recreational opportunities within the office building (table tennis, etc.) •	Training opportunities •	Attractive working environment and secure workplace •	Free coffee and fruit days •	Various career options</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -863,12 +867,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Budapest 10. ker.</t>
+          <t>Budapest 11. ker.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2709 Ft/óra</t>
+          <t>2200-2800 Ft/óra</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -880,44 +884,14 @@
       <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>muisz</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Student for IT Support &amp; Virtual Integration Tester</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>https://muisz.hu/diakmunkaink/IT-support-trainee%20-xi-kerulet--28247</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Student for IT Support &amp; Virtual Integration Tester Today the community of around 1800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. Join a dynamic and innovative team that is shaping the future of surgical imaging! We are developing a cutting-edge framework that enables C-arms to seamlessly integrate and run surgical software applications without compromising core functionality. You’ll work in a colocated development team, while collaborating with an international business network.  You will have the opportunity to learn and contribute to the development of a market-leading product that is already making a real impact in healthcare. If you love technology, problem-solving, and making an impact in healthcare, this is your chance! Feladatok •	Assist with system testing and installations. •	Work with Windows environments, including PowerShell scripting and basic network configuration. •	Support the setup and troubleshooting of our virtual integration testing environment. •	Contribute to improvements and maintenance of virtualization solutions (preferably Hyper-V, or similar technologies). •	Collaborate on tasks involving C#/.NET development for integration and automation purposes. Elvárások •	Ongoing university studies in a realated filed. •	Solid understanding of Windows OS and PowerShell. •	Basic knowledge of networking concepts. •	Experience with virtualization platforms (Hyper-V or similar). •	Familiarity with C#/.NET is a strong advantage. •	Problem-solving mindset and willingness to learn new technologies. Egyéb What we offer: •	Hybrid work model: 3 days/week home office opportunity (on average) •	Flexible working hours •	A young, dynamic, supporting team with mentor •	Attractive working environment and secure workplace •	Opportunity for international work experience •	Training possibilities: Language, soft-skill and technical trainings, corporate programs, meetups •	Various career opportunities •	Loyalty programs (Siemens Share Matching Program and Company loan opportunity) •	You can join several communities: sport, CSR, Go green, ToastMasters, etc. •	Family Friendly Workplace</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>magyar, angol</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Budapest 11. ker.</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2200-2800 Ft/óra</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -926,60 +900,102 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>muisz</t>
+          <t>schonherz</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Test framework developer trainee</t>
+          <t>Manuális Tesztelő Gyakornok</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/Test-framework-developer-trainee%20-xi-kerulet--28240</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40888-manualis-tesztelo-gyakornok</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Test framework developer trainee “Today the community of around 1,800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems, and you can even find them/us in electric cars. There are hardly any industrial areas where the programs our colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members 30 years ago. As of today, our headcount has nearly reached 1,800 employees and we are expanding – join us, be part of our team!” We are looking for a new colleague who will join our office in Budapest: Feladatok •	Implement and write tests for Angular web applications •	Work in a team and actively communicate with members •	Be able to work independently Elvárások •	Ongoing higher education studies (software engineering or similar) •	Angular or React experience •	Communication level English •	Have strong understanding of programming paradigms •	Good communication and problem-solving skills, systems thinking Egyéb Advantages: •	Software development experience in Web applications •	Experience in UI automation •	DevOps experience What we offer: •	A young, dynamic, supporting team with mentor(s) •	Thesis topic and writing opportunity with an in-house consultant •	Home Office opportunity, flexible working hours •	Recreational opportunities within the office building (table tennis, etc.) •	Training opportunities •	Attractive working environment and secure workplace •	Free coffee and fruit days •	Various career options</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>magyar, angol</t>
-        </is>
-      </c>
+          <t>🏢 Partnerünk 2003-ban alakult, a munkatársak és vezetők tulajdonában álló, 170 fős vállalat stabil üzleti és pénzügyi háttérrel, több mint 50 visszatérő nagyvállalati ügyféllel.  Üzleti problémák támogatására fejlesztenek ki és vezetnek be alkalmazásokat, valamint üzemeltetik azokat hosszú távon. Az üzleti folyamatautomatizáció a legerősebb megkülönböztető jegyük. ⚡️ Partnerünk programjában sok újdonságot fogsz megismerni. Teljes körű tag leszel az egyik csapatunkban, ahol éles üzleti környezetben kapott feladatokon keresztül megtapasztalhatod, hogy milyen egy komplex, nagyvállalati projektben, szolgáltatásban dolgozni. A Program első hónapja a tanulásról szól online tananyagok és terület specifikus gyakorló feladatok segítségével.   Ezután egy sikeres értékelő beszélgetést követően bekerülsz egy projekt csapatba, ahol már éles gyakorlati projektekben, szolgáltatásokban fejlesztheted tovább tudásodat, valós ügyfél feladatokat megoldva. Feladatok: ✨ Egyedi fejlesztésű üzleti alkalmazások tesztelési feladatainak ellátása (funkcionális, integrációs és end-to-end tesztelés) ✨ Részvétel tesztforgatókönyvek elkészítésében ✨ Manuális tesztelési feladatok végrehajtása, teszteredmények dokumentálása ✨ Hibák dokumentálása, javítások visszatesztelése ✨ Közreműködés a hibakezelési és változáskezelési folyamatokban a fejlesztési projektek során ✨ Együttműködés üzleti elemzőkkel és fejlesztőkkel Elvárások: 🟣 Folyamatban lévő egyetemi vagy főiskolai tanulmányok informatikai területen, aktív vagy passzív (amennyiben még nem múltál el 25 éves) nappali tagozaton, minimum további 1 teljes évig 🟣 Informatikai megoldások iránti nyitottság 🟣 Alaposság, önálló munkavégzésre való képesség és csapatmunkában való részvétel 🟣 Hosszú távú elköteleződés a szoftvertesztelés iránt 🟣 Minimum 4 hónap tesztelői munkatapasztalat Amit Partnerünk kínál: 🌱 Rendszeres teljesítményértékelő és célkitűző beszélgetések, ahol a vezetővel közösen tekintitek át a szakmai fejlődést és karrierutat 🤝 Dedikált mentor támogatása, aki végigkíséri a szakmai fejlődést 📊 Versenyképes, mély szakmai tudás megszerzése nagyvállalati, üzletkritikus rendszereken végzett munka során 🎓 Szakmai vizsgák megszerzésének támogatása 📚 Tudásmélyítési lehetőség Udemy kurzusokon keresztül 🌟 Innovatív, inspiráló és barátságos munkakörnyezet ⏰ Munkaidő: Hibrid munkavégzés lehetősége betanulás után, általános 08:00-17:00 között ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Budapest 11. ker.</t>
+          <t>Budapest, XI. kerület + Home Office</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2200-2800 Ft/óra</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+          <t>Br. 2400 Ft/óra*</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>ml_score=5, ml_prob=0.43347392851310385</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.4334739285131038</v>
+      </c>
+      <c r="L12" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>schonherz</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Qlik Sense és adatbázis fejlesztő gyakornok</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40887-qlik-sense-es-adatbazis-fejleszto-gyakornok</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>🏬 Partnerünk technológiai megoldásokat tervez és gyárt nemzetközi ügyfelek számára az autóiparban, szórakoztatóelektronikában és vállalati szektorban. Termékkínálatuk magában foglalja a connected car rendszereket, audio- és vizuáltechnikai eszközöket, automatizált vállalati megoldásokat és egyéb infokommunikációs rendszereket. Rendszereik több mint 25 millió járműben találhatók meg világszerte, és neves nemzetközi márkákkal működnek együtt. 🌕 A Qlik Sense és adatbázis fejlesztő gyakornok a vállalat beszerzési, gyártási, illetve az ellátási lánc kezdeményezéseit támogató adatinfrastruktúra és elemzési képességek fejlesztéséért lesz felelős. A mérnöki, gyártási és beszerzési csapatokkal együttműködve a terület biztosítja a vállalat beszerzési vezető pozíciójának eléréséhez szükséges eszközöket, elemzési módszereket és adatokat. Feladatok: ✨ Segítségnyújtás belső és külső adatforrásokból álló adatbázisok létrehozásában, többek között a beszerzés, a költségmodellezés, a beszállítói menedzsment, a kereslet-előrejelzés, a fogyasztáselemzés és a gyártási elemzés támogatása érdekében ✨ Együttműködés a csapaton belüli és kívüli csoportokkal komplex, termelési szintű adatmodellek, riportok, szabványok, architektúrák, rendszerek és folyamatok tervezésében és fejlesztésében ✨ Olyan robusztus, megbízható és naprakész rendszerek, adatok és jelentések kialakításának támogatása, amelyek nagy mértékben skálázhatók és hosszú távon is fenntarthatók Elvárások: 🟣 Folyamatban lévő alap- vagy mesterszakos tanulmányok számítástechnika, adatelemzés, statisztika, mesterséges intelligencia, információs rendszerek vagy mérnöki területen 🟣 Adatbázis-technológiák szakmai ismerete, beleértve az SQL használatát 🟣 Egyetemi vagy szakmai tapasztalat relációs adatbázisok tervezésében és karbantartásában, felhőalapú szervereken 🟣 Jártasság üzleti intelligencia és döntéstámogató rendszerek használatában (pl. Qlik Sense, Tableau, Power BI) 🟣 Eredményorientált, erősen analitikus problémamegoldó szemlélet 🟣 Erős folyamatorientáltság, új folyamatok fejlesztésének és dokumentálásának képessége 🟣 Jó időmenedzsment készségek, projektek tervezése és végrehajtása meghatározott időkereten belül 🟣 Képesség keresztfunkcionális környezetben történő munkavégzésre és együttműködésre több csapattal (IT, beszerzés, tervezés, gyártás) 🟣 Kiváló kommunikációs és interperszonális készségek, csapatjátékos hozzáállás globális, mátrixszervezetben 🟣 Alkalmazkodóképesség a változó igényekhez és feltételekhez 🟣 Középfokú angol nyelvtudás szóban és írásban Amit Partnerünk kínál: 🌍 Nemzetközi környezetben szerezhető munkatapasztalat 📈 Fejlődési lehetőségek és önálló munkavégzés 🏙️ Könnyen megközelíthető irodaház 👥 Fiatalos, nyitott és jó hangulatú csapat 🎓 Lehetőség szakmai gyakorlat elvégzésére 🚀 Karrierépítési és hosszú távú munkalehetőség ⏰ Munkaidő: általános, 08:00-17:00 között, betanulás után hibrid munkavégzés lehetséges: 50% iroda 50% Home Office arányban ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Angol (középfok)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Budapest, XIII. kerület</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Br. 2500 Ft/óra*</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>ml_score=5, ml_prob=0.4340323111115782</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>5</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.4340323111115782</v>
+      </c>
+      <c r="L13" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -989,44 +1005,48 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Manuális Tesztelő Gyakornok</t>
+          <t>Full-stack fejlesztő</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40888-manualis-tesztelo-gyakornok</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40885-full-stack-fejleszto</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🏢 Partnerünk 2003-ban alakult, a munkatársak és vezetők tulajdonában álló, 170 fős vállalat stabil üzleti és pénzügyi háttérrel, több mint 50 visszatérő nagyvállalati ügyféllel.  Üzleti problémák támogatására fejlesztenek ki és vezetnek be alkalmazásokat, valamint üzemeltetik azokat hosszú távon. Az üzleti folyamatautomatizáció a legerősebb megkülönböztető jegyük. ⚡️ Partnerünk programjában sok újdonságot fogsz megismerni. Teljes körű tag leszel az egyik csapatunkban, ahol éles üzleti környezetben kapott feladatokon keresztül megtapasztalhatod, hogy milyen egy komplex, nagyvállalati projektben, szolgáltatásban dolgozni. A Program első hónapja a tanulásról szól online tananyagok és terület specifikus gyakorló feladatok segítségével.   Ezután egy sikeres értékelő beszélgetést követően bekerülsz egy projekt csapatba, ahol már éles gyakorlati projektekben, szolgáltatásokban fejlesztheted tovább tudásodat, valós ügyfél feladatokat megoldva. Feladatok: ✨ Egyedi fejlesztésű üzleti alkalmazások tesztelési feladatainak ellátása (funkcionális, integrációs és end-to-end tesztelés) ✨ Részvétel tesztforgatókönyvek elkészítésében ✨ Manuális tesztelési feladatok végrehajtása, teszteredmények dokumentálása ✨ Hibák dokumentálása, javítások visszatesztelése ✨ Közreműködés a hibakezelési és változáskezelési folyamatokban a fejlesztési projektek során ✨ Együttműködés üzleti elemzőkkel és fejlesztőkkel Elvárások: 🟣 Folyamatban lévő egyetemi vagy főiskolai tanulmányok informatikai területen, aktív vagy passzív (amennyiben még nem múltál el 25 éves) nappali tagozaton, minimum további 1 teljes évig 🟣 Informatikai megoldások iránti nyitottság 🟣 Alaposság, önálló munkavégzésre való képesség és csapatmunkában való részvétel 🟣 Hosszú távú elköteleződés a szoftvertesztelés iránt 🟣 Minimum 4 hónap tesztelői munkatapasztalat Amit Partnerünk kínál: 🌱 Rendszeres teljesítményértékelő és célkitűző beszélgetések, ahol a vezetővel közösen tekintitek át a szakmai fejlődést és karrierutat 🤝 Dedikált mentor támogatása, aki végigkíséri a szakmai fejlődést 📊 Versenyképes, mély szakmai tudás megszerzése nagyvállalati, üzletkritikus rendszereken végzett munka során 🎓 Szakmai vizsgák megszerzésének támogatása 📚 Tudásmélyítési lehetőség Udemy kurzusokon keresztül 🌟 Innovatív, inspiráló és barátságos munkakörnyezet ⏰ Munkaidő: Hibrid munkavégzés lehetősége betanulás után, általános 08:00-17:00 között ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
+          <t>🏢 Partnerünk Magyarország egyik legmodernebb vendéglátó szoftverének fejlesztő cége. Céljuk nemcsak az, hogy rendszerük egyszerűen használható, gyors és megbízható legyen, hanem az is, hogy minden kapcsolódó szolgáltatásuk kimagasló színvonalat képviseljen. Mindezzel felfrissítve és megreformálva a vendéglátás területét. Feladatok: 🎮 Termékfejlesztés, bekapcsolódás a tervezésbe 🎮 Új funkciók fejlesztése 🎮 Meglévő funkciók továbbfejlesztése, kiegészítése 🎮 Új technológiák kipróbálása, beépítése a fejlesztési folyamatba 🎮 Visszajelzések kezelése, problémák megoldása, hibajavítás 🎮 Fejlesztői csapat munkájának támogatása 🎮 Aktív részvétel a projektekben és a szoftverek minőségének folyamatos javításában Elvárások: 🧩 Folyamatban lévő végzéshez közeli informatikai tanulmányok 🧩 Önéletrajz a korábbi tapasztalatok részletes megjelölésével, ha van 🧩 Minimum középfokú angol nyelvtudás 🧩 Verziókezelő szoftverek ismerete (pl: Git) 🧩 Java, Javascipt programozási nyelv ismerete és gyakorlat a használatában 🧩 Kódolási szabványok és best practice-ek követése 🧩 Igényes a kódjára és szeret megoldani, nem csak “megcsinálni” 🧩 Hozzáállásában proaktív, megoldásközpontú 🧩 Jó kommunikációs képesség, jó megjelenés 🧩 Monotonitástűrés, pontosság 🧩 Erős problémamegoldó gondolkodás (hibakeresés, root cause, kreatív megoldások) 🧩 Rendszerszintű szemlélet 🧩 Önállóság és ownership (feladat végigvitele, felelősségvállalás) 🧩 Csapatban való jó együttműködés (code review, közös döntések) 🧩 Nyitottság a tanulásra és a fejlődésre ⏰ Munkaidő: 09:00 - 17:00. Home Office-ra nincs lehetőség. ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Angol középfok</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Budapest, XI. kerület + Home Office</t>
+          <t>Budapest XIII. kerület</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Br. 2400 Ft/óra*</t>
+          <t>Br. 2145 Ft/óra*</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>ml_score=5, ml_prob=0.43347392851310385</t>
+          <t>ml_score=4, ml_prob=0.3944167289469815</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K14" t="n">
-        <v>0.4334739285131038</v>
+        <v>0.3944167289469815</v>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -1037,45 +1057,45 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Qlik Sense és adatbázis fejlesztő gyakornok</t>
+          <t>Frontend Fejlesztő</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40887-qlik-sense-es-adatbazis-fejleszto-gyakornok</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40881-frontend-fejleszto</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>🏬 Partnerünk technológiai megoldásokat tervez és gyárt nemzetközi ügyfelek számára az autóiparban, szórakoztatóelektronikában és vállalati szektorban. Termékkínálatuk magában foglalja a connected car rendszereket, audio- és vizuáltechnikai eszközöket, automatizált vállalati megoldásokat és egyéb infokommunikációs rendszereket. Rendszereik több mint 25 millió járműben találhatók meg világszerte, és neves nemzetközi márkákkal működnek együtt. 🌕 A Qlik Sense és adatbázis fejlesztő gyakornok a vállalat beszerzési, gyártási, illetve az ellátási lánc kezdeményezéseit támogató adatinfrastruktúra és elemzési képességek fejlesztéséért lesz felelős. A mérnöki, gyártási és beszerzési csapatokkal együttműködve a terület biztosítja a vállalat beszerzési vezető pozíciójának eléréséhez szükséges eszközöket, elemzési módszereket és adatokat. Feladatok: ✨ Segítségnyújtás belső és külső adatforrásokból álló adatbázisok létrehozásában, többek között a beszerzés, a költségmodellezés, a beszállítói menedzsment, a kereslet-előrejelzés, a fogyasztáselemzés és a gyártási elemzés támogatása érdekében ✨ Együttműködés a csapaton belüli és kívüli csoportokkal komplex, termelési szintű adatmodellek, riportok, szabványok, architektúrák, rendszerek és folyamatok tervezésében és fejlesztésében ✨ Olyan robusztus, megbízható és naprakész rendszerek, adatok és jelentések kialakításának támogatása, amelyek nagy mértékben skálázhatók és hosszú távon is fenntarthatók Elvárások: 🟣 Folyamatban lévő alap- vagy mesterszakos tanulmányok számítástechnika, adatelemzés, statisztika, mesterséges intelligencia, információs rendszerek vagy mérnöki területen 🟣 Adatbázis-technológiák szakmai ismerete, beleértve az SQL használatát 🟣 Egyetemi vagy szakmai tapasztalat relációs adatbázisok tervezésében és karbantartásában, felhőalapú szervereken 🟣 Jártasság üzleti intelligencia és döntéstámogató rendszerek használatában (pl. Qlik Sense, Tableau, Power BI) 🟣 Eredményorientált, erősen analitikus problémamegoldó szemlélet 🟣 Erős folyamatorientáltság, új folyamatok fejlesztésének és dokumentálásának képessége 🟣 Jó időmenedzsment készségek, projektek tervezése és végrehajtása meghatározott időkereten belül 🟣 Képesség keresztfunkcionális környezetben történő munkavégzésre és együttműködésre több csapattal (IT, beszerzés, tervezés, gyártás) 🟣 Kiváló kommunikációs és interperszonális készségek, csapatjátékos hozzáállás globális, mátrixszervezetben 🟣 Alkalmazkodóképesség a változó igényekhez és feltételekhez 🟣 Középfokú angol nyelvtudás szóban és írásban Amit Partnerünk kínál: 🌍 Nemzetközi környezetben szerezhető munkatapasztalat 📈 Fejlődési lehetőségek és önálló munkavégzés 🏙️ Könnyen megközelíthető irodaház 👥 Fiatalos, nyitott és jó hangulatú csapat 🎓 Lehetőség szakmai gyakorlat elvégzésére 🚀 Karrierépítési és hosszú távú munkalehetőség ⏰ Munkaidő: általános, 08:00-17:00 között, betanulás után hibrid munkavégzés lehetséges: 50% iroda 50% Home Office arányban ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+          <t>🏬 Partnerünk valós idejű beltéri helymeghatározó rendszert kínál, amely gyártócsarnokokból származó adatokat biztosít az üzem optimalizálásához és a termelés ipar 4.0 szintre emeléséhez. A bevált technológiájukkal már kritikus problémákat oldottak meg Fortune 500-as vállalatok gyáraiban, miközben kisebb üzemek hatékonyságát is jelentősen növelték. Feladatok: 🔹 Partnerünk valós idejű pozícióadatokon alapuló szoftvermegoldásokat fejleszt nemzetközi gyártó- és logisztikai partnerek számára 🔹 A megoldások saját fejlesztésű, gyártott pozícionáló hardverekre és szoftverkomponensekre épülnek 🔹 A rendszer backend oldala Python (FastAPI), míg frontend oldala TypeScript (Angular) technológiával készült 🔹 A 10 fős, kis létszámú csapat jelenleg elsősorban alkalmazás-orientált, egyedi fejlesztésekre fókuszál 🔹 Ezen projektekhez keresnek új frontend fejlesztő gyakornokot, aki aktív részt vállal az egyedi alkalmazások kidolgozásában Elvárások: 🫐 Folyamatban lévő felsőfokú tanulmányok 🫐 TypeScript (Angular) ismerete és használatában szerzett tapasztalat 🫐 Angol nyelvtudás írásban 🫐 Jó problémamegoldó készség 🫐 Önálló, proaktív munkavégzés 🫐 Néhány fős fejlesztői csapatban való hatékony együttműködés Amit Partnerünk kínál: 🌎 Magyar tulajdonú kisvállalkozás 5 fős fejlesztői maggal és több részmunkaidős kollégával ⏰ Munkaidő: Törzsidő: 09:00-16:00, de rugalmasan beosztható ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Angol (középfok)</t>
+          <t>Angol (írásban)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Budapest, XIII. kerület</t>
+          <t>Budapest, X. kerület+ Home Office</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Br. 2500 Ft/óra*</t>
+          <t>Br. 2200 Ft/óra*</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>ml_score=5, ml_prob=0.4340323111115782</t>
+          <t>ml_score=5, ml_prob=0.4464931897180971</t>
         </is>
       </c>
       <c r="J15" t="n">
         <v>5</v>
       </c>
       <c r="K15" t="n">
-        <v>0.4340323111115782</v>
+        <v>0.4464931897180971</v>
       </c>
       <c r="L15" t="n">
         <v>5</v>
@@ -1089,45 +1109,45 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Full-stack fejlesztő</t>
+          <t>Junior Data Engineer Intern</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40885-full-stack-fejleszto</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40867-junior-data-engineer-intern</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>🏢 Partnerünk Magyarország egyik legmodernebb vendéglátó szoftverének fejlesztő cége. Céljuk nemcsak az, hogy rendszerük egyszerűen használható, gyors és megbízható legyen, hanem az is, hogy minden kapcsolódó szolgáltatásuk kimagasló színvonalat képviseljen. Mindezzel felfrissítve és megreformálva a vendéglátás területét. Feladatok: 🎮 Termékfejlesztés, bekapcsolódás a tervezésbe 🎮 Új funkciók fejlesztése 🎮 Meglévő funkciók továbbfejlesztése, kiegészítése 🎮 Új technológiák kipróbálása, beépítése a fejlesztési folyamatba 🎮 Visszajelzések kezelése, problémák megoldása, hibajavítás 🎮 Fejlesztői csapat munkájának támogatása 🎮 Aktív részvétel a projektekben és a szoftverek minőségének folyamatos javításában Elvárások: 🧩 Folyamatban lévő végzéshez közeli informatikai tanulmányok 🧩 Önéletrajz a korábbi tapasztalatok részletes megjelölésével, ha van 🧩 Minimum középfokú angol nyelvtudás 🧩 Verziókezelő szoftverek ismerete (pl: Git) 🧩 Java, Javascipt programozási nyelv ismerete és gyakorlat a használatában 🧩 Kódolási szabványok és best practice-ek követése 🧩 Igényes a kódjára és szeret megoldani, nem csak “megcsinálni” 🧩 Hozzáállásában proaktív, megoldásközpontú 🧩 Jó kommunikációs képesség, jó megjelenés 🧩 Monotonitástűrés, pontosság 🧩 Erős problémamegoldó gondolkodás (hibakeresés, root cause, kreatív megoldások) 🧩 Rendszerszintű szemlélet 🧩 Önállóság és ownership (feladat végigvitele, felelősségvállalás) 🧩 Csapatban való jó együttműködés (code review, közös döntések) 🧩 Nyitottság a tanulásra és a fejlődésre ⏰ Munkaidő: 09:00 - 17:00. Home Office-ra nincs lehetőség. ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+          <t>🌎 Our Partner is a supply chain software company, focusing on tools and data for Lifecycle Assessment (LCA) practitioners. 📍They are seeking a motivated Intern / Junior Data Engineer to join their team. This person will work on designing, building, and maintaining scalable data pipelines, contributing to their data infrastructure and enabling data-driven decision-making across the organization. Tasks ✨ Developing and implementing data models based on business requirements, with a focus on performance and scalability ✨ Designing, building, and maintaining scalable data pipelines, where experience with Apache Airflow is an advantage ✨ Implementing and maintaining Kafka-based streaming data pipelines for real-time data processing and system integration ✨ Integrating data pipelines with third-party databases and APIs ✨ Establishing monitoring, alerting, and maintenance procedures to ensure the reliability and health of data pipelines ✨ Collaborating with cross-functional teams, including data scientists, analysts, and stakeholders, to understand data requirements Requirements 🟣 Ongoing higher education studies in Computer Science, Software Engineering, or a related field 🟣 Proficiency in Python and SQL, with experience in data manipulation and transformation 🟣 Understanding of data warehouse concepts and data modeling techniques 🟣 Experience in designing, building, and maintaining data pipelines 🟣 Understanding of Kafka-based streaming architectures for real-time data processing 🟣 Confident and active written and spoken English knowledge, as the team collaborates in English 🟣 Ability to communicate effectively in a virtual, remote work environment Work Environment 🌍 Full remote work environment 🚀 Opportunity to gain hands-on experience in a fast-moving, innovative product environment 🧑‍🏫 Mentorship from experienced engineers, with guidance on best practices and effective testing approaches ⏰ Working hours: 📌 Flexible working hours 📌 Availability required for a few overlapping hours with the main team to support communication 📌 Occasional evening availability may be needed due to time zone differences ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Send us your english CV with a photo to the hr@schonherz.hu e-mail adress! * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 693 700 per month.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Angol középfok</t>
+          <t>English (Fluent)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Budapest XIII. kerület</t>
+          <t>Home Office</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Br. 2145 Ft/óra*</t>
+          <t>Gross 2700-3400 Ft/hour*</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>ml_score=4, ml_prob=0.3944167289469815</t>
+          <t>ml_score=4, ml_prob=0.36878801654730486</t>
         </is>
       </c>
       <c r="J16" t="n">
         <v>4</v>
       </c>
       <c r="K16" t="n">
-        <v>0.3944167289469815</v>
+        <v>0.3687880165473049</v>
       </c>
       <c r="L16" t="n">
         <v>4</v>
@@ -1141,48 +1161,48 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Frontend Fejlesztő</t>
+          <t>C++ Developer Intern</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40881-frontend-fejleszto</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40863-c-developer-intern</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>🏬 Partnerünk valós idejű beltéri helymeghatározó rendszert kínál, amely gyártócsarnokokból származó adatokat biztosít az üzem optimalizálásához és a termelés ipar 4.0 szintre emeléséhez. A bevált technológiájukkal már kritikus problémákat oldottak meg Fortune 500-as vállalatok gyáraiban, miközben kisebb üzemek hatékonyságát is jelentősen növelték. Feladatok: 🔹 Partnerünk valós idejű pozícióadatokon alapuló szoftvermegoldásokat fejleszt nemzetközi gyártó- és logisztikai partnerek számára 🔹 A megoldások saját fejlesztésű, gyártott pozícionáló hardverekre és szoftverkomponensekre épülnek 🔹 A rendszer backend oldala Python (FastAPI), míg frontend oldala TypeScript (Angular) technológiával készült 🔹 A 10 fős, kis létszámú csapat jelenleg elsősorban alkalmazás-orientált, egyedi fejlesztésekre fókuszál 🔹 Ezen projektekhez keresnek új frontend fejlesztő gyakornokot, aki aktív részt vállal az egyedi alkalmazások kidolgozásában Elvárások: 🫐 Folyamatban lévő felsőfokú tanulmányok 🫐 TypeScript (Angular) ismerete és használatában szerzett tapasztalat 🫐 Angol nyelvtudás írásban 🫐 Jó problémamegoldó készség 🫐 Önálló, proaktív munkavégzés 🫐 Néhány fős fejlesztői csapatban való hatékony együttműködés Amit Partnerünk kínál: 🌎 Magyar tulajdonú kisvállalkozás 5 fős fejlesztői maggal és több részmunkaidős kollégával ⏰ Munkaidő: Törzsidő: 09:00-16:00, de rugalmasan beosztható ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+          <t>🚗 Our Partner is a software development company specializing in autonomous vehicles. Their primary approach to self-driving technology is camera-based, relying on image processing, while also experimenting with radar and lidar solutions. The company is Hungarian-owned, yet operates with a distinctly American-style, relaxed management culture, works on numerous U.S.-based projects, and offers internal career advancement opportunities. Tasks: 🚗 Working on the next-generation vehicle self-driving software ⚙️ Development of the internal data distribution and execution framework 🔌 Integration of third-party frameworks 🧠 Development of interfaces to aiSim (in-house sensor and vehicle simulator) 📡 Sensor data recording–related tasks 🖥️ Development of human–machine interfaces and data visualization tools 🤝 Applying social competency, flexibility, and effective collaboration with developer and research teams 🚙 Working with different automotive platforms 🔬 Close cooperation with other developer and research teams Requirements: 🎓 Ongoing (active or passive) full-time university studies for at least one more year ⏳ Availability of at least 20 working hours per week 💻 Advanced knowledge of C++ 🌍 Intermediate level of English 🎯 Precise, reliable and quality-focused attitude 🚀 Independent and proactive mindset What our Partner offers: 💼 Possibility to gain valuable work experience at the forefront of the hardware development sector 💰 Competitive student salary 🌟 Inspiring and supportive working environment 🤝 Teambuilding events and additional benefits for students ⏰ Flexible working hours 📈 Long-term job opportunity 🚀 Possibility of an immediate start 🎓 In-service training opportunity 🏋️ Fitness opportunities 🍽️ Free lunch every workday at one of the best all-you-can-eat restaurants in Budapest or delivered by Wolt for Work ⏰ Working hours: between 08:00 and 18:00 🏠 Home office possibility after the onboarding period, in a 50–50% hybrid arrangement ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Send us your english CV with a photo to the hr@schonherz.hu e-mail adress! * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 693 700 per month.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Angol (írásban)</t>
+          <t>English (intermediate)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Budapest, X. kerület+ Home Office</t>
+          <t>Budapest District II. + Home Office</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Br. 2200 Ft/óra*</t>
+          <t>Gross 2250–2500 HUF/hour*</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>ml_score=5, ml_prob=0.4464931897180971</t>
+          <t>ml_score=3, ml_prob=0.2765983513284454</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K17" t="n">
-        <v>0.4464931897180971</v>
+        <v>0.2765983513284454</v>
       </c>
       <c r="L17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1193,97 +1213,97 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Junior Data Engineer Intern</t>
+          <t>Junior szoftverfejlesztő gyakornok</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40867-junior-data-engineer-intern</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40850-junior-szoftverfejleszto-gyakornok</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>🌎 Our Partner is a supply chain software company, focusing on tools and data for Lifecycle Assessment (LCA) practitioners. 📍They are seeking a motivated Intern / Junior Data Engineer to join their team. This person will work on designing, building, and maintaining scalable data pipelines, contributing to their data infrastructure and enabling data-driven decision-making across the organization. Tasks ✨ Developing and implementing data models based on business requirements, with a focus on performance and scalability ✨ Designing, building, and maintaining scalable data pipelines, where experience with Apache Airflow is an advantage ✨ Implementing and maintaining Kafka-based streaming data pipelines for real-time data processing and system integration ✨ Integrating data pipelines with third-party databases and APIs ✨ Establishing monitoring, alerting, and maintenance procedures to ensure the reliability and health of data pipelines ✨ Collaborating with cross-functional teams, including data scientists, analysts, and stakeholders, to understand data requirements Requirements 🟣 Ongoing higher education studies in Computer Science, Software Engineering, or a related field 🟣 Proficiency in Python and SQL, with experience in data manipulation and transformation 🟣 Understanding of data warehouse concepts and data modeling techniques 🟣 Experience in designing, building, and maintaining data pipelines 🟣 Understanding of Kafka-based streaming architectures for real-time data processing 🟣 Confident and active written and spoken English knowledge, as the team collaborates in English 🟣 Ability to communicate effectively in a virtual, remote work environment Work Environment 🌍 Full remote work environment 🚀 Opportunity to gain hands-on experience in a fast-moving, innovative product environment 🧑‍🏫 Mentorship from experienced engineers, with guidance on best practices and effective testing approaches ⏰ Working hours: 📌 Flexible working hours 📌 Availability required for a few overlapping hours with the main team to support communication 📌 Occasional evening availability may be needed due to time zone differences ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Send us your english CV with a photo to the hr@schonherz.hu e-mail adress! * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 693 700 per month.</t>
+          <t>💼 Partnerünk egy egy univerzális platform, amely egyetlen felületen egyesíti a töltőhálózatokat és intelligensen ajánlja a legjobb töltési lehetőségeket a felhasználóknak. A csapat fiatal, dinamikus, startup szemléletű, ahol a hallgató közvetlenül senior fejlesztőktől tanulhat, és valós termékbe kerülő feladatokon dolgozhat. 👉 A diák a fejlesztői csapat munkáját támogatja kisebb programozási, tesztelési és technikai előkészítő feladatokkal. A napi munkavégzés során önállóan és iránymutatások alapján is el tudja látni a rá bízott részfeladatokat. A pozíció célja, hogy a hallgató ipari környezetben szerezzen gyakorlati tapasztalatot, és hozzájáruljon a termékek fejlesztéséhez. Feladatok: 🐻‍❄️ Kisebb fejlesztési feladatok elvégzése JavaScript-ben (helper funkciók, API-hívások, adatfeldolgozó modulok) 🐻‍❄️ Hibák reprodukálása, logok elemzése és hibaokok azonosítása fejlesztői útmutatás alapján 🐻‍❄️ Mobil- és webalkalmazás manuális tesztelése különböző eszközökön, tesztelési jegyzőkönyvek vezetése 🐻‍❄️ API válaszok ellenőrzése (JSON struktúrák értelmezése, adatösszehasonlítás) 🐻‍❄️ Egyszerűbb Node.js vagy frontend komponensek módosítása (a tudásszinttől függően) 🐻‍❄️ Dokumentációk frissítése (Confluence), tesztelési scenariók és technikai jegyzetek készítése 🐻‍❄️ A fejlesztői workflow támogatása: Jira ticketek előkészítése, adatok rendszerezése 🐻‍❄️ Adatellenőrzési feladatok (árak, töltőpont adatok, API kimenetek validálása) 🐻‍❄️ Kisebb UI/UX észrevételek gyűjtése, képernyőképek készítése és rendszerezése 🐻‍❄️ Fejlesztők támogatása egyszerűbb szoftveres kutató- vagy összehasonlító feladatokkal Elvárások: 📗 Folyamatban lévő mérnökinformatikus, mechatronikai mérnök, vagy villamosmérnök tanulmányok, még legalább 1 féléven keresztül 📗 Magabiztos JavaScript-ismeret 📗 Alapszintű Git használat 📗 JSON és REST API működésének megértése 📗 Önálló, precíz munkavégzés 📗 Rendszerszintű, logikus gondolkodás 📗 Heti minimum 1 nap irodai jelenlét vállalása 📗 Önéletrajz munkatapasztalat megjelölésével 📗 Angol középfokú nyelvtudás 📗 Pontosság, precizitás 📗 Jó kommunikációs készség 📗 Önálló, felelősségteljes munkavégzés 📗 Proaktív hozzáállás és problémamegoldó készség 📗 Csapatmunkára való alkalmasság Előnyök: 🔻 Mobilalkalmazás-fejlesztési tapasztalat 🔻 UI/UX érzék, Figma ismerete 🔻 Korábbi szoftverfejlesztési projekt vagy gyakornoki tapasztalat 🔻 Elektromobilitási vagy energetikai tapasztalat, ismeret 🔻 B kategóriás jogosítvány Amit Partnerünk kínál: 🏡 A diák heti 1 alkalommal a budapesti irodában, a hét további részében pedig Home Office-ban dolgozhat 🛜 Az iroda modern, ergonomikus munkaállomásokkal, gyors internettel és fejlesztői eszközökkel felszerelt 💡 A csapat fiatal, innovatív, együttműködő, senior backend- és frontend-fejlesztőkből áll, akik támogatják a betanulást ✅ A cég értékei: átlátható kommunikáció, minőségi fejlesztés, gyors iteráció és adatvezérelt gondolkodás ✏️ A munkát modern eszközök (GitHub, Jira, Confluence, fejlesztői környezetek) segítik, időszakos csapatépítőkkel és tudásmegosztásokkal ⏰ Munkaidő: 09:00-17:00 között, az otthoni munkavégzés rugalmas időbeosztásban működik, Partner osztja be a feladatokat ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>English (Fluent)</t>
+          <t>Angol (Középfok)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Home Office</t>
+          <t>Budapest, VI. kerület + Home Office</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Gross 2700-3400 Ft/hour*</t>
+          <t>Br. 2300-2500 Ft/óra*</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>ml_score=4, ml_prob=0.36878801654730486</t>
+          <t>ml_score=5, ml_prob=0.44376624117112995</t>
         </is>
       </c>
       <c r="J18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K18" t="n">
-        <v>0.3687880165473049</v>
+        <v>0.4437662411711299</v>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>schonherz</t>
+          <t>muisz</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>C++ Developer Intern</t>
+          <t>Technical Writer</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40863-c-developer-intern</t>
+          <t>https://muisz.hu/diakmunkaink/technical-writer-budapest-13-ker--26725</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚗 Our Partner is a software development company specializing in autonomous vehicles. Their primary approach to self-driving technology is camera-based, relying on image processing, while also experimenting with radar and lidar solutions. The company is Hungarian-owned, yet operates with a distinctly American-style, relaxed management culture, works on numerous U.S.-based projects, and offers internal career advancement opportunities. Tasks: 🚗 Working on the next-generation vehicle self-driving software ⚙️ Development of the internal data distribution and execution framework 🔌 Integration of third-party frameworks 🧠 Development of interfaces to aiSim (in-house sensor and vehicle simulator) 📡 Sensor data recording–related tasks 🖥️ Development of human–machine interfaces and data visualization tools 🤝 Applying social competency, flexibility, and effective collaboration with developer and research teams 🚙 Working with different automotive platforms 🔬 Close cooperation with other developer and research teams Requirements: 🎓 Ongoing (active or passive) full-time university studies for at least one more year ⏳ Availability of at least 20 working hours per week 💻 Advanced knowledge of C++ 🌍 Intermediate level of English 🎯 Precise, reliable and quality-focused attitude 🚀 Independent and proactive mindset What our Partner offers: 💼 Possibility to gain valuable work experience at the forefront of the hardware development sector 💰 Competitive student salary 🌟 Inspiring and supportive working environment 🤝 Teambuilding events and additional benefits for students ⏰ Flexible working hours 📈 Long-term job opportunity 🚀 Possibility of an immediate start 🎓 In-service training opportunity 🏋️ Fitness opportunities 🍽️ Free lunch every workday at one of the best all-you-can-eat restaurants in Budapest or delivered by Wolt for Work ⏰ Working hours: between 08:00 and 18:00 🏠 Home office possibility after the onboarding period, in a 50–50% hybrid arrangement ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Send us your english CV with a photo to the hr@schonherz.hu e-mail adress! * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 693 700 per month.</t>
+          <t>Technical Writer Technical Writer position for trainee. Feladatok •	Objectives of the service: o	Develop comprehensive Knowledge Base documentation that meets organizational ITSM standards o	Gain deep understanding of services and processes, and translate complex information into simple, polished, engaging content o	Write user-friendly content that meets the needs of target audience, turning insights into language for user success o	Develop and maintain detailed database of reference materials o	Based on user’s feedback develop innovative methods for improvement •	The responsibilities of the Technical Writer cover the following services: o	Research, outline, write, and edit content, working closely with IT Service departments to understand processes and services provided by the department o	Gather information from subject-matter experts and develop, organize, and write Knowledge Base articles based on procedure manuals, process documentations. o	Work with development and support leads to identify documentation repositories, revise and edit, and determine best solutions for data compilation and centralized storage o	Research, create, and maintain knowledge based documentation templates that adhere to organizational and legal standards and allow for easy navigation and search for information o	Develop content for maximum usability, with consistent voice across all documentation o	Report to IT Service Management of the company o	Create and maintain reports with Grafana o	Organize meetings to promote the completed materials o	IT Service Onboarding process support Elvárások - experience in Technical Writer work (about 6-12 months) - ongoing studies in IT/economics/technology/engineering - fluency in English, both written and spoken - an interest and/or experience in IT - This would be a 35-40 hours per week position with hybrid working. Home office 2-3 days per week</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>English (intermediate)</t>
+          <t>magyar, angol</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Budapest District II. + Home Office</t>
+          <t>Budapest 13. ker.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Gross 2250–2500 HUF/hour*</t>
+          <t>2200-2500 Ft/óra</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.2765983513284454</t>
+          <t>ml_score=3, ml_prob=0.2353742789808101</t>
         </is>
       </c>
       <c r="J19" t="n">
         <v>3</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2765983513284454</v>
+        <v>0.2353742789808101</v>
       </c>
       <c r="L19" t="n">
         <v>3</v>
@@ -1292,53 +1312,53 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>schonherz</t>
+          <t>muisz</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Junior szoftverfejlesztő gyakornok</t>
+          <t>Begyázott rendszereket tesztelő gyakornok</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40850-junior-szoftverfejleszto-gyakornok</t>
+          <t>https://muisz.hu/diakmunkaink/beagyazott-rendszertesztelo-bp-xi-kerulet--28286</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>💼 Partnerünk egy egy univerzális platform, amely egyetlen felületen egyesíti a töltőhálózatokat és intelligensen ajánlja a legjobb töltési lehetőségeket a felhasználóknak. A csapat fiatal, dinamikus, startup szemléletű, ahol a hallgató közvetlenül senior fejlesztőktől tanulhat, és valós termékbe kerülő feladatokon dolgozhat. 👉 A diák a fejlesztői csapat munkáját támogatja kisebb programozási, tesztelési és technikai előkészítő feladatokkal. A napi munkavégzés során önállóan és iránymutatások alapján is el tudja látni a rá bízott részfeladatokat. A pozíció célja, hogy a hallgató ipari környezetben szerezzen gyakorlati tapasztalatot, és hozzájáruljon a termékek fejlesztéséhez. Feladatok: 🐻‍❄️ Kisebb fejlesztési feladatok elvégzése JavaScript-ben (helper funkciók, API-hívások, adatfeldolgozó modulok) 🐻‍❄️ Hibák reprodukálása, logok elemzése és hibaokok azonosítása fejlesztői útmutatás alapján 🐻‍❄️ Mobil- és webalkalmazás manuális tesztelése különböző eszközökön, tesztelési jegyzőkönyvek vezetése 🐻‍❄️ API válaszok ellenőrzése (JSON struktúrák értelmezése, adatösszehasonlítás) 🐻‍❄️ Egyszerűbb Node.js vagy frontend komponensek módosítása (a tudásszinttől függően) 🐻‍❄️ Dokumentációk frissítése (Confluence), tesztelési scenariók és technikai jegyzetek készítése 🐻‍❄️ A fejlesztői workflow támogatása: Jira ticketek előkészítése, adatok rendszerezése 🐻‍❄️ Adatellenőrzési feladatok (árak, töltőpont adatok, API kimenetek validálása) 🐻‍❄️ Kisebb UI/UX észrevételek gyűjtése, képernyőképek készítése és rendszerezése 🐻‍❄️ Fejlesztők támogatása egyszerűbb szoftveres kutató- vagy összehasonlító feladatokkal Elvárások: 📗 Folyamatban lévő mérnökinformatikus, mechatronikai mérnök, vagy villamosmérnök tanulmányok, még legalább 1 féléven keresztül 📗 Magabiztos JavaScript-ismeret 📗 Alapszintű Git használat 📗 JSON és REST API működésének megértése 📗 Önálló, precíz munkavégzés 📗 Rendszerszintű, logikus gondolkodás 📗 Heti minimum 1 nap irodai jelenlét vállalása 📗 Önéletrajz munkatapasztalat megjelölésével 📗 Angol középfokú nyelvtudás 📗 Pontosság, precizitás 📗 Jó kommunikációs készség 📗 Önálló, felelősségteljes munkavégzés 📗 Proaktív hozzáállás és problémamegoldó készség 📗 Csapatmunkára való alkalmasság Előnyök: 🔻 Mobilalkalmazás-fejlesztési tapasztalat 🔻 UI/UX érzék, Figma ismerete 🔻 Korábbi szoftverfejlesztési projekt vagy gyakornoki tapasztalat 🔻 Elektromobilitási vagy energetikai tapasztalat, ismeret 🔻 B kategóriás jogosítvány Amit Partnerünk kínál: 🏡 A diák heti 1 alkalommal a budapesti irodában, a hét további részében pedig Home Office-ban dolgozhat 🛜 Az iroda modern, ergonomikus munkaállomásokkal, gyors internettel és fejlesztői eszközökkel felszerelt 💡 A csapat fiatal, innovatív, együttműködő, senior backend- és frontend-fejlesztőkből áll, akik támogatják a betanulást ✅ A cég értékei: átlátható kommunikáció, minőségi fejlesztés, gyors iteráció és adatvezérelt gondolkodás ✏️ A munkát modern eszközök (GitHub, Jira, Confluence, fejlesztői környezetek) segítik, időszakos csapatépítőkkel és tudásmegosztásokkal ⏰ Munkaidő: 09:00-17:00 között, az otthoni munkavégzés rugalmas időbeosztásban működik, Partner osztja be a feladatokat ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+          <t>Begyázott rendszereket tesztelő gyakornok A Siemens Mobility Kft. K+F központjában, a XI. kerületi Infoparkban olyan projekteken dolgozunk, melyek biztosítják a zavartalan, fenntartható, megbízható és biztonságos közlekedést. Tudj meg többet a cégünkről: https://www.mobility.siemens.com/hu/hu.html Feladatok •	Vasúti járművek vezérlőrendszerének tesztelése •	Tesztautomatizálási forgatókönyvek írása Behave keretrendszerrel (BDD) •	Verziókezelés SVN segítségével •	CI/CD folyamatok támogatása Jenkins környezetben •	Hibák dokumentálása, riportálása, együttműködés fejlesztőkkel és tesztelőkkel Elvárások •	Heti 25 óra munkavállalása •	Python nyelv magabiztos ismerete •	Tesztelési szemlélet, BDD alapok ismerete előny •	Csapatmunkára való nyitottság, precizitás •	Legalább középszintű angol nyelvtudás (írásban és szóban) •	Aktív hallgatói jogviszony (informatikai vagy műszaki területen) Egyéb Előnyt jelent: •	Tapasztalat Behave, SVN, Jenkins használatában •	Automatizált tesztelési tapasztalat (pl. Selenium, pytest) •	Magabiztos német nyelvtudás (szóban és írásban) Amit kínálunk: •	Valós projektekben való részvétel nemzetközi környezetben •	Szakmai fejlődési lehetőség •	Rugalmas munkaidő, otthoni munkavégzés lehetősége</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Angol (Középfok)</t>
+          <t>magyar, angol</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Budapest, VI. kerület + Home Office</t>
+          <t>Budapest 11. ker.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Br. 2300-2500 Ft/óra*</t>
+          <t>2700 Ft/óra</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>ml_score=5, ml_prob=0.44376624117112995</t>
+          <t>ml_score=3, ml_prob=0.2677280832564894</t>
         </is>
       </c>
       <c r="J20" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K20" t="n">
-        <v>0.4437662411711299</v>
+        <v>0.2677280832564894</v>
       </c>
       <c r="L20" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1349,17 +1369,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Technical Writer</t>
+          <t>Test Engineer Trainee</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/technical-writer-budapest-13-ker--26725</t>
+          <t>https://muisz.hu/diakmunkaink/Test-Engineer-trainee%20-xi-kerulet--28335</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Technical Writer Technical Writer position for trainee. Feladatok •	Objectives of the service: o	Develop comprehensive Knowledge Base documentation that meets organizational ITSM standards o	Gain deep understanding of services and processes, and translate complex information into simple, polished, engaging content o	Write user-friendly content that meets the needs of target audience, turning insights into language for user success o	Develop and maintain detailed database of reference materials o	Based on user’s feedback develop innovative methods for improvement •	The responsibilities of the Technical Writer cover the following services: o	Research, outline, write, and edit content, working closely with IT Service departments to understand processes and services provided by the department o	Gather information from subject-matter experts and develop, organize, and write Knowledge Base articles based on procedure manuals, process documentations. o	Work with development and support leads to identify documentation repositories, revise and edit, and determine best solutions for data compilation and centralized storage o	Research, create, and maintain knowledge based documentation templates that adhere to organizational and legal standards and allow for easy navigation and search for information o	Develop content for maximum usability, with consistent voice across all documentation o	Report to IT Service Management of the company o	Create and maintain reports with Grafana o	Organize meetings to promote the completed materials o	IT Service Onboarding process support Elvárások - experience in Technical Writer work (about 6-12 months) - ongoing studies in IT/economics/technology/engineering - fluency in English, both written and spoken - an interest and/or experience in IT - This would be a 35-40 hours per week position with hybrid working. Home office 2-3 days per week</t>
+          <t>Test Engineer Trainee “Today the community of around 1,800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems, and you can even find them/us in electric cars. There are hardly any industrial areas where the programs our colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members 30 years ago. As of today, our headcount has nearly reached 1,800 employees and we are expanding – join us, be part of our team!” Feladatok The candidate's task: •	The Test Engineer trainee is responsible for the support of planning, execution and documentation of the Train IT tests, according to norms and specifications within the specified time frame. Main tasks: •	Preparation of the tests incl. test environment •	Execution of the tests according to the test instructions •	Analysis on any identified deviations from expected results and their possible causes •	Documentation of the tests carried out, the tests environment and the test conditions •	Testing mechanical hardware, electrical hardware and software Elvárások Competence: •	Testing methodology •	Analytical skills and solution-oriented •	Structured and systematic approach •	English knowledge Egyéb What we offer: •	A young, dynamic, supporting team with mentor(s) •	Thesis topic and writing opportunity with an in-house consultant •	Home Office opportunity, flexible working hours •	Recreational opportunities within the office building (table football, table tennis) •	Free training opportunities •	Attractive working environment and secure workplace •	Free coffee and fruit days •	Various career options Not required but a plus: •	Python knowledge (target level: basic) •	Git and Svn •	Behaviour Driven Development approach</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1369,25 +1389,25 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Budapest 13. ker.</t>
+          <t>Budapest 11. ker.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2200-2500 Ft/óra</t>
+          <t>2200-2800 Ft/óra</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.2353742789808101</t>
+          <t>ml_score=3, ml_prob=0.2087337787498741</t>
         </is>
       </c>
       <c r="J21" t="n">
         <v>3</v>
       </c>
       <c r="K21" t="n">
-        <v>0.2353742789808101</v>
+        <v>0.2087337787498741</v>
       </c>
       <c r="L21" t="n">
         <v>3</v>
@@ -1401,17 +1421,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Begyázott rendszereket tesztelő gyakornok</t>
+          <t>Test Automation Framework Developer Trainee</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/beagyazott-rendszertesztelo-bp-xi-kerulet--28286</t>
+          <t>https://muisz.hu/diakmunkaink/Test-Automation-Framework-xi-kerulet--28211</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Begyázott rendszereket tesztelő gyakornok A Siemens Mobility Kft. K+F központjában, a XI. kerületi Infoparkban olyan projekteken dolgozunk, melyek biztosítják a zavartalan, fenntartható, megbízható és biztonságos közlekedést. Tudj meg többet a cégünkről: https://www.mobility.siemens.com/hu/hu.html Feladatok •	Vasúti járművek vezérlőrendszerének tesztelése •	Tesztautomatizálási forgatókönyvek írása Behave keretrendszerrel (BDD) •	Verziókezelés SVN segítségével •	CI/CD folyamatok támogatása Jenkins környezetben •	Hibák dokumentálása, riportálása, együttműködés fejlesztőkkel és tesztelőkkel Elvárások •	Heti 25 óra munkavállalása •	Python nyelv magabiztos ismerete •	Tesztelési szemlélet, BDD alapok ismerete előny •	Csapatmunkára való nyitottság, precizitás •	Legalább középszintű angol nyelvtudás (írásban és szóban) •	Aktív hallgatói jogviszony (informatikai vagy műszaki területen) Egyéb Előnyt jelent: •	Tapasztalat Behave, SVN, Jenkins használatában •	Automatizált tesztelési tapasztalat (pl. Selenium, pytest) •	Magabiztos német nyelvtudás (szóban és írásban) Amit kínálunk: •	Valós projektekben való részvétel nemzetközi környezetben •	Szakmai fejlődési lehetőség •	Rugalmas munkaidő, otthoni munkavégzés lehetősége</t>
+          <t>Test Automation Framework Developer Trainee “Today the community of around 1800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems and you can even find them/us in electric cars. There are hardly any industrial areas where the programs I and my colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members more than 30 years ago. As of today, our headcount has reached the 1800 employees and we are expanding – join us, be part of our team!” We are looking for a new colleague who will join our office in Budapest: Feladatok The main objective of the project is to support the development of the SINAMICS frequency converter product lineup by providing a test automation hardware and software suite. We provide the means to learn the necessary project specific skills during training. •	Operate and maintain fully automated test equipment and commission new installations •	Integrate test equipment with the test automation system •	Manage project hardware inventory •	Hardware procurement •	Maintain contact with our suppliers •	Actively participate in an Agile (Scrum) team •	Regular contact with colleagues in Germany (In German or in English) Elvárások •	Ongoing studies in a related field •	Basic electronics and electrical engineering knowledge •	Willingness to perform work in an electrical laboratory •	Openness to learning new technologies •	Minimum basic level German and English knowledge Egyéb Advantages: •	Experience reading electrical circuit diagrams •	Electrical assembly experience •	Electrical measurement experience •	Industrial automation knowledge •	PLC programming knowledge •	Drive system knowledge (Siemens Sinamics devices) What we offer: •	Home office opportunity and flexible working hours •	Closed, guarded parking area •	A young, dynamic, supporting team with mentor •	Attractive working environment and secure workplace •	Various career opportunities •	You can join several communities: sport, CSR, Go green, ToastMasters, etc. •	Family Friendly Workplace</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1426,20 +1446,20 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2700 Ft/óra</t>
+          <t>2200-2800 Ft/óra</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.2677280832564894</t>
+          <t>ml_score=3, ml_prob=0.212769145498217</t>
         </is>
       </c>
       <c r="J22" t="n">
         <v>3</v>
       </c>
       <c r="K22" t="n">
-        <v>0.2677280832564894</v>
+        <v>0.212769145498217</v>
       </c>
       <c r="L22" t="n">
         <v>3</v>
@@ -1453,17 +1473,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Test Engineer Trainee</t>
+          <t>Business Analyst</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/Test-Engineer-trainee%20-xi-kerulet--28335</t>
+          <t>https://muisz.hu/diakmunkaink/business-analyst-budapest-iii-kerulet--28274</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Test Engineer Trainee “Today the community of around 1,800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems, and you can even find them/us in electric cars. There are hardly any industrial areas where the programs our colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members 30 years ago. As of today, our headcount has nearly reached 1,800 employees and we are expanding – join us, be part of our team!” Feladatok The candidate's task: •	The Test Engineer trainee is responsible for the support of planning, execution and documentation of the Train IT tests, according to norms and specifications within the specified time frame. Main tasks: •	Preparation of the tests incl. test environment •	Execution of the tests according to the test instructions •	Analysis on any identified deviations from expected results and their possible causes •	Documentation of the tests carried out, the tests environment and the test conditions •	Testing mechanical hardware, electrical hardware and software Elvárások Competence: •	Testing methodology •	Analytical skills and solution-oriented •	Structured and systematic approach •	English knowledge Egyéb What we offer: •	A young, dynamic, supporting team with mentor(s) •	Thesis topic and writing opportunity with an in-house consultant •	Home Office opportunity, flexible working hours •	Recreational opportunities within the office building (table football, table tennis) •	Free training opportunities •	Attractive working environment and secure workplace •	Free coffee and fruit days •	Various career options Not required but a plus: •	Python knowledge (target level: basic) •	Git and Svn •	Behaviour Driven Development approach</t>
+          <t>Business Analyst A Greenventions Kft. több mint 10 éve van jelen a technológiai innováció területén, és számos sikeres rendszerintegrációs projektet valósított meg. Csatlakozz hozzánk és legyél részese egy dinamikus csapatnak, ahol a szakmai fejlődés és a megbecsülés alapértékek Feladatok -	Üzleti igények összegyűjtésének támogatása: részvétel megbeszéléseken, jegyzetelés, információk rendszerezése -	Interfész specifikációk, architektúra ábrák készítése -	Workshopok előkészítése és támogatása: kérdések összeállítása, témák strukturálása, dokumentálás -	Backlog karbantartásában való részvétel: user story-k egyszerűsítése, priorizálás támogatása -	Koncepcionális és funkcionális tervezés támogatása: folyamatábrák, logikai modellek készítésének támogatása -	UX/UI tervezési feladatok támogatása: képernyővázlatok készítése egyszerűbb feladatokra, felhasználói visszajelzések összegzése -	Tesztelések és élesítési folyamatok támogatása: tesztforgatókönyvek összeállítása, eredmények dokumentálása Elvárások -	BME informatika vagy Corvinus gazdinfo vagy Corvinus közgáz végzős hallgatói státusz -	Heti 32–40 óra vállalása -	Minimális BA vagy rendszerszervezői munkatapasztalat -	Erős technikai beállítottság, nyitottság az IT rendszerek működésének megértésére -	Analitikus gondolkodás, rendszerszemlélet, logikus feladatmegközelítés -	Agilis módszertanok alapszintű ismerete vagy nyitottság azok megtanulására -	Alapvető affinitás szoftverfejlesztési projektek iránt Egyéb Munkaidő: - 9-17h - tudunk rugalmasak lenni egyetemi elfoglaltság esetén - Alkalomszerűen Home Office is megoldható Heti minimum óraszám: - 32-40 óra Bruttó bér: - 3500-4000Ft / óra - tapasztalati szinttől függően,</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1473,25 +1493,25 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Budapest 11. ker.</t>
+          <t>Budapest 3. ker.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2200-2800 Ft/óra</t>
+          <t>3500-4000 Ft/óra</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.2087337787498741</t>
+          <t>ml_score=3, ml_prob=0.2689983234312848</t>
         </is>
       </c>
       <c r="J23" t="n">
         <v>3</v>
       </c>
       <c r="K23" t="n">
-        <v>0.2087337787498741</v>
+        <v>0.2689983234312848</v>
       </c>
       <c r="L23" t="n">
         <v>3</v>
@@ -1505,17 +1525,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Test Automation Framework Developer Trainee</t>
+          <t>Beágyazott Szoftverfejlesztő Gyakornok</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/Test-Automation-Framework-xi-kerulet--28211</t>
+          <t>https://muisz.hu/diakmunkaink/beagyazott-szoftverfejleszto-gyakornok-budapest-xxiii-kerulet--23962</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Test Automation Framework Developer Trainee “Today the community of around 1800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems and you can even find them/us in electric cars. There are hardly any industrial areas where the programs I and my colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members more than 30 years ago. As of today, our headcount has reached the 1800 employees and we are expanding – join us, be part of our team!” We are looking for a new colleague who will join our office in Budapest: Feladatok The main objective of the project is to support the development of the SINAMICS frequency converter product lineup by providing a test automation hardware and software suite. We provide the means to learn the necessary project specific skills during training. •	Operate and maintain fully automated test equipment and commission new installations •	Integrate test equipment with the test automation system •	Manage project hardware inventory •	Hardware procurement •	Maintain contact with our suppliers •	Actively participate in an Agile (Scrum) team •	Regular contact with colleagues in Germany (In German or in English) Elvárások •	Ongoing studies in a related field •	Basic electronics and electrical engineering knowledge •	Willingness to perform work in an electrical laboratory •	Openness to learning new technologies •	Minimum basic level German and English knowledge Egyéb Advantages: •	Experience reading electrical circuit diagrams •	Electrical assembly experience •	Electrical measurement experience •	Industrial automation knowledge •	PLC programming knowledge •	Drive system knowledge (Siemens Sinamics devices) What we offer: •	Home office opportunity and flexible working hours •	Closed, guarded parking area •	A young, dynamic, supporting team with mentor •	Attractive working environment and secure workplace •	Various career opportunities •	You can join several communities: sport, CSR, Go green, ToastMasters, etc. •	Family Friendly Workplace</t>
+          <t>Beágyazott Szoftverfejlesztő Gyakornok Beágyazott szoftverfejlesztői csapatunk biztonságkritikus vasúti fékvezérlő egységek szoftverének fejlesztésével foglalkozik. Ebbe a csapatba keresünk egy lelkes gyakornokot aki munkájával hozzájárulna a sikeres fejlesztéshez. A kiírt feladatokat lehetőség van egyben szakmai gyakorlat, szakdolgozat vagy diplomamunka keretében is elvégezni. Feladatok Milyen feladatok várnak rád? •	Szoftverkomponensek implementálása fékvezérlő elektronikai egységekhez a követelményeknek és az architektúrának megfelelően •	Részvétel technikai felülvizsgálatokban •	Kapcsolódó dokumentációk készítése és karbantartása •	A fejlesztést támogató alkalmazások fejlesztése •	Rendszerintegráció és -konfiguráció támogatása Elvárások Te vagy számunkra a megfelelő munkatárs, ha: •	Felsőfokú műszaki tanulmányaid folytatod •	C programnyelvet ismered •	Angol nyelvtudásod szívesen használod •	Strukturált gondolkodásmód jellemez Egyéb MIÉRT VÁLASSZ MINKET? •	Rugalmas időbeosztásban a tanulmányaid mellett tudsz dolgozni •	Szakmai gyakorlat, szakdolgozat, diploma elvégzésének lehetősége •	Barátságos és támogató csapat vár rád •	Később akár főállásban is dolgozhatsz nálunk •	Extrák: céges konditerem, parkolási lehetőség, vállalati rendezvények, képzések •	Megismerhetsz egy nemzetközi vállalatot és annak tevékenységét •	Az itt szerzett tudásod garantáltan értékes lesz a munkaerőpiacon</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1525,25 +1545,25 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Budapest 11. ker.</t>
+          <t>Budapest 23. ker.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2200-2800 Ft/óra</t>
+          <t>2390 Ft/óra</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.212769145498217</t>
+          <t>ml_score=3, ml_prob=0.26319210848731006</t>
         </is>
       </c>
       <c r="J24" t="n">
         <v>3</v>
       </c>
       <c r="K24" t="n">
-        <v>0.212769145498217</v>
+        <v>0.2631921084873101</v>
       </c>
       <c r="L24" t="n">
         <v>3</v>
@@ -1552,53 +1572,55 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>muisz</t>
+          <t>schonherz</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Business Analyst</t>
+          <t>Rendszermérnök gyakornok</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/business-analyst-budapest-iii-kerulet--28274</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40847-rendszermernok-gyakornok</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Business Analyst A Greenventions Kft. több mint 10 éve van jelen a technológiai innováció területén, és számos sikeres rendszerintegrációs projektet valósított meg. Csatlakozz hozzánk és legyél részese egy dinamikus csapatnak, ahol a szakmai fejlődés és a megbecsülés alapértékek Feladatok -	Üzleti igények összegyűjtésének támogatása: részvétel megbeszéléseken, jegyzetelés, információk rendszerezése -	Interfész specifikációk, architektúra ábrák készítése -	Workshopok előkészítése és támogatása: kérdések összeállítása, témák strukturálása, dokumentálás -	Backlog karbantartásában való részvétel: user story-k egyszerűsítése, priorizálás támogatása -	Koncepcionális és funkcionális tervezés támogatása: folyamatábrák, logikai modellek készítésének támogatása -	UX/UI tervezési feladatok támogatása: képernyővázlatok készítése egyszerűbb feladatokra, felhasználói visszajelzések összegzése -	Tesztelések és élesítési folyamatok támogatása: tesztforgatókönyvek összeállítása, eredmények dokumentálása Elvárások -	BME informatika vagy Corvinus gazdinfo vagy Corvinus közgáz végzős hallgatói státusz -	Heti 32–40 óra vállalása -	Minimális BA vagy rendszerszervezői munkatapasztalat -	Erős technikai beállítottság, nyitottság az IT rendszerek működésének megértésére -	Analitikus gondolkodás, rendszerszemlélet, logikus feladatmegközelítés -	Agilis módszertanok alapszintű ismerete vagy nyitottság azok megtanulására -	Alapvető affinitás szoftverfejlesztési projektek iránt Egyéb Munkaidő: - 9-17h - tudunk rugalmasak lenni egyetemi elfoglaltság esetén - Alkalomszerűen Home Office is megoldható Heti minimum óraszám: - 32-40 óra Bruttó bér: - 3500-4000Ft / óra - tapasztalati szinttől függően,</t>
+          <t>Partnerünk nagyvállalati IT rendszerek üzembe helyezésével, üzemeltetésével és támogatásával foglalkozik. A cég üzemeltető csapatába keres tapasztalt kollégát Linux alapú rendszerek, valamint vállalati folyamatokat támogató (Enterprise Service Management) rendszer üzemeltetésére. Feladatok: 💻 Linux alapú infrastruktúra szolgáltatások konfigurálása, üzemeltetése (pl. SUSE Linux Enterprise Server, Prometheus, Grafana, Icinga, reverse proxy, adatbázisok, egyéb nagyvállalati rendszerek) 💻 Enterprise Service Management eszközben folyamatok, adatmodellek, integrációs csatornák tervezése, kialakítása, módosítási igények teljesítése 💻 Üzemeltetés- és projekttámogatási munkálatokban, implementációban, dokumentálási és hibaelhárítási tevékenységben való részvétel 💻 A felmerülő problémák megoldása önállóan és távoli támogatás segítségével 💻 Az implementációhoz és támogatáshoz szükséges termék- és rendszerismeretek elsajátítása 💻 Csapaton belüli együttműködés és ehhez szükséges mértékű és minőségű kommunikáció Elvárások: 🎓 Folyamatban lévő felsőfokú tanulmányok 📚 Legalább 3 elvégzett félév informatikai szakterületen 🐧 Erős érdeklődés és tapasztalat Linux környezetben 💻 Jártasság szkriptnyelvekben vagy programozási nyelvekben 🌍 Középfokú angol nyelvvizsga vagy azzal egyenértékű angol nyelvtudás 🗣️ Kiváló kommunikációs készség szóban és írásban, ügyfélbarát hozzáállás 🎯 Precizitás, alaposság és igényesség kreatív és monoton feladatok esetén egyaránt 📈 Új ismeretek gyors elsajátítására való igény és készség Előny: 💻 Szkriptnyelvekben vagy programozási nyelvekben szerzett mélyebb tapasztalat 🎓 Felsőfokú informatikai végzettség ☸️ Kubernetes tapasztalat 🌍 Felsőfokú angol nyelvtudás Amit a Partnerünk kínál: 🏢 Nagyvállalati tapasztalat megszerzésének lehetősége 🚀 Komoly kihívást és szakmai fejlődést biztosító feladatok 🤝 Segítőkész, magasan kvalifikált szakmai csapat ⚡ Együttműködő és dinamikus közösség 🏢 Modern irodai munkakörülmények 🏠 Távoli munkavégzés lehetősége ⏰ Munkaidő: az ügyfél munkarendjéhez igazodó munkavégzés 🕗 Munkaidőkeret: 08:00–18:00 ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>magyar, angol</t>
+          <t>Angol (középszint)</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Budapest 3. ker.</t>
+          <t>Budapest XIII. kerület, XI. kerület, VII. kerület</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>3500-4000 Ft/óra</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
+          <t>Br. 2200-2600 Ft/óra*</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.2689983234312848</t>
+          <t>ml_score=4, ml_prob=0.3024948970959473</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K25" t="n">
-        <v>0.2689983234312848</v>
+        <v>0.3024948970959473</v>
       </c>
       <c r="L25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1609,45 +1631,47 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Beágyazott Szoftverfejlesztő Gyakornok</t>
+          <t>IT Support Specialist Trainee</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/beagyazott-szoftverfejleszto-gyakornok-budapest-xxiii-kerulet--23962</t>
+          <t>https://muisz.hu/diakmunkaink/it-support-specialist-trainee-budapest-3-ker--28030</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Beágyazott Szoftverfejlesztő Gyakornok Beágyazott szoftverfejlesztői csapatunk biztonságkritikus vasúti fékvezérlő egységek szoftverének fejlesztésével foglalkozik. Ebbe a csapatba keresünk egy lelkes gyakornokot aki munkájával hozzájárulna a sikeres fejlesztéshez. A kiírt feladatokat lehetőség van egyben szakmai gyakorlat, szakdolgozat vagy diplomamunka keretében is elvégezni. Feladatok Milyen feladatok várnak rád? •	Szoftverkomponensek implementálása fékvezérlő elektronikai egységekhez a követelményeknek és az architektúrának megfelelően •	Részvétel technikai felülvizsgálatokban •	Kapcsolódó dokumentációk készítése és karbantartása •	A fejlesztést támogató alkalmazások fejlesztése •	Rendszerintegráció és -konfiguráció támogatása Elvárások Te vagy számunkra a megfelelő munkatárs, ha: •	Felsőfokú műszaki tanulmányaid folytatod •	C programnyelvet ismered •	Angol nyelvtudásod szívesen használod •	Strukturált gondolkodásmód jellemez Egyéb MIÉRT VÁLASSZ MINKET? •	Rugalmas időbeosztásban a tanulmányaid mellett tudsz dolgozni •	Szakmai gyakorlat, szakdolgozat, diploma elvégzésének lehetősége •	Barátságos és támogató csapat vár rád •	Később akár főállásban is dolgozhatsz nálunk •	Extrák: céges konditerem, parkolási lehetőség, vállalati rendezvények, képzések •	Megismerhetsz egy nemzetközi vállalatot és annak tevékenységét •	Az itt szerzett tudásod garantáltan értékes lesz a munkaerőpiacon</t>
+          <t>IT Support Specialist Trainee Graphisoft® empowers teams to design great buildings through award-winning software solutions, learning programs, and professional services for the AEC industry. Our award-winning products and solutions support OPEN BIM for workflow transparency, longevity, and data accessibility for built assets.  Archicad®, the architects’ BIM software of choice, offers a complete end-to-end design and documentation workflow for architectural and integrated architectural and engineering practices of any size. BIMx®, the most popular mobile and web BIM app, extends the BIM experience to include all stakeholders in the building design, delivery, and operations lifecycle. BIMcloud®, the AEC industry’s first and most advanced cloud-based team collaboration solution, makes real-time collaboration possible across the globe regardless of the size of the project and the speed or quality of the team members’ network connection. DDScad solutions support users with intelligent Mechanical, Electrical, and Plumbing (MEP) design tools, integrated calculations, and comprehensive documentation of all building system disciplines. Graphisoft is part of the Nemetschek Group. To learn more, visit more visit www.graphisoft.com Feladatok •	Provide on-site support in the Budapest office and assist with basic remote support for colleagues worldwide, in both English and Hungarian. •	Assist in end-user support for PCs, Macs, mobile devices (iOS and Android), printers, scanners, and video conferencing systems. •	Support colleagues in the effective use of collaboration platforms such as Microsoft Teams, SharePoint Online, and Miro. •	Participate in basic system administration tasks (Active Directory, Microsoft 365) under the guidance of senior team members. •	Provide first-level application support for Microsoft Teams, Outlook, Word, Excel, and PowerPoint. •	Help with incident and service request ticket handling: categorization, documentation, and updating users on progress. •	Contribute to maintaining user guides, FAQs, and process documentation. •	Assist with hardware asset tracking and lifecycle processes. •	Participate in basic network troubleshooting (DNS, DHCP, IP) with guidance from experienced colleagues. •	Gain exposure to emerging technologies and contribute ideas for improvements. Elvárások •	Ongoing studies in IT field at a Hungarian university. •	Active student status for at least 2 semesters. •	Proficiency in both English and Hungarian. •	Eagerness to learn and openness to new technologies. •	Customer-oriented mindset and willingness to respond quickly to requests. •	A minimum of 20 hours of work per week. •	Team player with a proactive and problem-solving attitude. •	Motivation to help others and build practical IT skills. Egyéb •	International, inspiring, and dynamic environment. •	Challenging and various tasks. •	Continuous learning &amp; development opportunities. •	The flexibility of a hybrid workplace with at least 1 day / week home office (after the probationary period). If you think this description fits you, come and join us in our company headquarters located at the well-known Graphisoft Park!</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>magyar, angol</t>
+          <t>magyar</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Budapest 23. ker.</t>
+          <t>Budapest 3. ker.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2390 Ft/óra</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
+          <t>2005 Ft/ óra</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.26319210848731006</t>
+          <t>ml_score=3, ml_prob=0.23130507951893228</t>
         </is>
       </c>
       <c r="J26" t="n">
         <v>3</v>
       </c>
       <c r="K26" t="n">
-        <v>0.2631921084873101</v>
+        <v>0.2313050795189323</v>
       </c>
       <c r="L26" t="n">
         <v>3</v>
@@ -1656,37 +1680,33 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>schonherz</t>
+          <t>muisz</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Rendszermérnök gyakornok</t>
+          <t>Programozás oktatása (XI. kerület)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40847-rendszermernok-gyakornok</t>
+          <t>https://muisz.hu/diakmunkaink/programozas-oktatasa-xi-kerulet-budapest-xi-kerulet--12147</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Partnerünk nagyvállalati IT rendszerek üzembe helyezésével, üzemeltetésével és támogatásával foglalkozik. A cég üzemeltető csapatába keres tapasztalt kollégát Linux alapú rendszerek, valamint vállalati folyamatokat támogató (Enterprise Service Management) rendszer üzemeltetésére. Feladatok: 💻 Linux alapú infrastruktúra szolgáltatások konfigurálása, üzemeltetése (pl. SUSE Linux Enterprise Server, Prometheus, Grafana, Icinga, reverse proxy, adatbázisok, egyéb nagyvállalati rendszerek) 💻 Enterprise Service Management eszközben folyamatok, adatmodellek, integrációs csatornák tervezése, kialakítása, módosítási igények teljesítése 💻 Üzemeltetés- és projekttámogatási munkálatokban, implementációban, dokumentálási és hibaelhárítási tevékenységben való részvétel 💻 A felmerülő problémák megoldása önállóan és távoli támogatás segítségével 💻 Az implementációhoz és támogatáshoz szükséges termék- és rendszerismeretek elsajátítása 💻 Csapaton belüli együttműködés és ehhez szükséges mértékű és minőségű kommunikáció Elvárások: 🎓 Folyamatban lévő felsőfokú tanulmányok 📚 Legalább 3 elvégzett félév informatikai szakterületen 🐧 Erős érdeklődés és tapasztalat Linux környezetben 💻 Jártasság szkriptnyelvekben vagy programozási nyelvekben 🌍 Középfokú angol nyelvvizsga vagy azzal egyenértékű angol nyelvtudás 🗣️ Kiváló kommunikációs készség szóban és írásban, ügyfélbarát hozzáállás 🎯 Precizitás, alaposság és igényesség kreatív és monoton feladatok esetén egyaránt 📈 Új ismeretek gyors elsajátítására való igény és készség Előny: 💻 Szkriptnyelvekben vagy programozási nyelvekben szerzett mélyebb tapasztalat 🎓 Felsőfokú informatikai végzettség ☸️ Kubernetes tapasztalat 🌍 Felsőfokú angol nyelvtudás Amit a Partnerünk kínál: 🏢 Nagyvállalati tapasztalat megszerzésének lehetősége 🚀 Komoly kihívást és szakmai fejlődést biztosító feladatok 🤝 Segítőkész, magasan kvalifikált szakmai csapat ⚡ Együttműködő és dinamikus közösség 🏢 Modern irodai munkakörülmények 🏠 Távoli munkavégzés lehetősége ⏰ Munkaidő: az ügyfél munkarendjéhez igazodó munkavégzés 🕗 Munkaidőkeret: 08:00–18:00 ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Angol (középszint)</t>
-        </is>
-      </c>
+          <t>Programozás oktatása (XI. kerület) Jelentkezz nálunk egy érdekes és izgalmas munkára! LOGISCOOL BUDA-ÚJBUDA Programozás speciális, élmény alapú tanítására keresünk egyetemistákat, 16 év feletti középiskolásokat. Feladatok Iskolánk a Logiscool Buda-Újbuda, ( a központ cím: 1116 Budapest, Fehérvári út 108-112, és 1122 Budapest, Maros utca 12.) A tanítás 2025 szeptemberében kezdődik és folyamatosan tart az iskolai tanévekhez igazodva budai és újbudai területeken. Rugalmasan választható, órarendhez igazíthatóan tudsz nálunk csoportokat vállalni. Óráinkat a központi iskolánkban minden hétköznap délutánonként 14:00 - 18:30 óra között, valamint szombaton délelőtt tartjuk a 1,5-1,5 órás foglalkozásokat.  A kihelyezett helyszíneken budán és újbudán is hétköznapokon akár 13:00 tól is már kezdődnek foglalkozásaink. Rugalmasan lehetőséged van egy vagy több napot hetente, vagy 1 vagy több csoportot naponta kiválasztani a tanításra – bármelyiket, amelyik Neked megfelel. Előzetesen oktatóinknak tréninget tartunk. Elvárások Ha •	nyitott vagy gyerekek oktatására, esetleg tanítási tapasztalataid vannak, •	kiváló kommunikációs készséggel rendelkezel és jó előadó vagy, •	kedveled a gyerekeket és szót is tudsz érteni velük, •	informatikai, programozói ismeretekkel rendelkezel, (előny, de nem feltétel) •	jó megjelenésű, határozott fellépésű, érdekes személyiség vagy, aki példaképül is szolgálhat, •	a kreativitás nem áll messze tőled, •	megbízható és pontos vagy, •	ismered az angol nyelvet, akkor várunk, jelentkezz nálunk! Egyéb Megfelelő díjazást: nettó 2.000 – 2.500 Ft órabér, (minimum 2000.-Ft + bónusz az elvégzett feladatok teljesítménye alapján), hosszú távú lehetőséget, rugalmas, órarendhez igazítható kellemes munkakörülményeket kínálunk egy fiatal csapatban. Kölcsönös elégedettség esetén dolgozhatsz nálunk majd nyári táborainkban is!</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Budapest XIII. kerület, XI. kerület, VII. kerület</t>
+          <t>Budapest 11. ker.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Br. 2200-2600 Ft/óra*</t>
+          <t>2000-2500 Ft/ óra</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1694,17 +1714,17 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>ml_score=4, ml_prob=0.3024948970959473</t>
+          <t>ml_score=3, ml_prob=0.26474386097465424</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K27" t="n">
-        <v>0.3024948970959473</v>
+        <v>0.2647438609746542</v>
       </c>
       <c r="L27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1715,32 +1735,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Szoftverfejlesztő</t>
+          <t>Frontend fejlesztő</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40776-szoftverfejleszto</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40729-frontend-fejleszto</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Partnerünk egy információszolgáltatással foglalkozó technológiai vállalat, amely az üzleti technológiákra specializálódik. Rendszerintegrációval, tanácsadással és szoftverfejlesztéssel nyújtanak IT-szolgáltatásokat. A szerver-, hálózati-, egységes kommunikációs technológiák és a szoftverfejlesztés területén szerzett mély szakértelmünkkel segítünk vállalkozásodnak növekedni és fejlődni a kitűzött célokkal összhangban. Hiszünk abban, hogy egyszerre tehetjük vállalkozásodat egyszerűbbé és hatékonyabbá. 💼 Egyszerre több projekt van folyamatban. A projekteken a kollégák csapatban dolgoznak, és egy vezető fejlesztő koordinálja a munkát. 🎯 Figyelembe veszik, hogy kinek mi az erőssége, illetve mely területek érdeklik jobban, és ennek megfelelően osztják le a feladatokat. 🌱 Többnyire univerzális munkatársakat keresnek, akik nyitottak a fejlődésre és tanulásra, és a preferált programozási területükön kívül más területeken is rendelkeznek alapszintű tudással. 🧭 A belépést követően egy tesztfeladatsoron kell végigmenni, amely pár hétig tart. Ez idő alatt megismerik a cég főbb szakmai irányvonalait, és egy kijelölt mentor segíti őket. Feladatok: ⬛️ Szoftverfejlesztés ⬛️ Részvétel az üzemeltetési feladatokban 💻 Használt backend technológiák: Java Quarkus, Java Spring, NodeJS Használt frontend technológiák: VueJS, Angular. Nem baj, ha nem ismered mindet, de légy nyitott más programnyelvek elsajátítására is. Elvárások: ✔️ Folyamatban lévő felsőfokú tanulmányok, lehetőleg végzéshez közel ✔️ Linux alapismeretek ✔️ Java programozási nyelv magabiztos ismerete ✔️ 3 félév elvégzése a megfelelő felsőoktatási programban vagy szakmai tapasztalat ✔️ Angol aktív szövegértés/szóbeli kommunikáció, írásban kevésbé használatos ✔️ Heti minimum 32 óra várható munkavégzés ✔️ Munkatapasztalat megjelölése, leírása ✔️ Referencia munka-link küldése ✔️ Motivációs levél ✔️ Legyen MySQL és minimális hálózati ismereted ✔️ Partnerrel történő találkozás során elegáns, hivatalos megjelenés ✔️ Önálló munkavégzésre való törekvés ✔️ Megbízhatóság ✔️ Csapatmunka ✔️ Precizitás ✔️ Pontosság ✔️ Határidők betartása ✔️ Jogosítvány nem feltétel, de megléte esetén a későbbiekben cégautó használat lehetősége fennáll Amit Partnerünk kínál: 🏡 14. kerületi családias lakásiroda, bogrács és medence is a rendelkezésre áll. 🇭🇺 Magyar tulajdonban lévő vállalkozás. 👨‍💻 Az Ügyvezető, egyben tulajdonos IT területről érkezett, részt vesz folyamatosan a projektekben. 🅿️ Utcán a parkolás ingyenes 🌳 Zugló kertvárosi részén, 3 emeletes villa kerttel, medencével 🎯 A pince klubhelyiséggé lett kialakítva (csocsó, pingpong, darts) 🤝 Családias hangulat, kb. 20 fő alkalmazott 🧑‍🎓 Átlag életkor 30 év alatti, egyetem mellett dolgozó, egyetemet végző, friss diplomás kollégák, szoftverfejlesztők 🎉 Rendszeres csapatépítők, bográcsozás, vetélkedős estek. Az irodában kávé, tea, víz, sós és édes és egyéb szezonnak megfelelő nassolnivalók a rendelkezésre állnak Hosszútávú munkalehetőség, a tanulmányok után főállású pozíció is elnyerhető. 📚 Nem csak a szakmai gyakorlatod leigazolásában, de akár a szakdolgozatodban is szívesen segítünk. 📅 Munkaidő: Kötetlen munkarend ⏰ Törzsidő : 9:00-16:00 Alapvetően irodai munkavégzés, az első 3-6 hónapban biztosan bejárós, de ha önállóan tudsz dolgozni, akkor 1-2 nap HO is oké a későbbiekben. ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+          <t>🏢 Partnerünk átfogó szoftverfejlesztéssel foglalkozik, egészen a tervezéstől a karbantartásig. Felhőalapú megoldásaikkal hatékonyabbá, biztonságosabbá és fenntarthatóbbá teszik a vállalkozásokat. Feladatok: 🧩 Fejlesztési feladatok: 📝 Webes/cross-platform applikációk fejlesztése főként vállalati portálokhoz, oktatási rendszerekhez a legújabb technológiákban (Vue, React, React Native) 📝 Cloud architechtúra alapú fejlesztések 📝 Friss, gyors átfutási idővel (3-6 hónap / projekt) rendelkező projektek 📝 Rugalmasan oszthatod be a munkaóráid 🧩Adminisztratív teendőkhöz: 📝 GitLab-en rögzített teendőid áttekintése, elvégzése 📝 Kérdések esetén egyeztetés, könnyen, gyorsan, Teams-en Elvárások: 🎯 Folyamatban lévő felsőfokú tanulmányok 🎯 Vue.js ÉS React ismeret 🎯 Az önéletrajz kézhezvételét követően próbafeladat megoldása szükséges 🎯 Angol társalgási szintű nyelvtudás 🎯 Informatikai beállítottság, pontosság Munkakörnyezet: 🏢 Home Office lehetőség 🏢 Igény esetén a III. kerületi irodában is biztosított a munkavégzés (nem kötelező) ⏰ Munkaidő: Kötetlen ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami 693 700 Ft havonta.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Angol (Középfok)</t>
+          <t>Angol társalgási szint</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Budapest XIV. kerület</t>
+          <t>Home office</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Br. 2200-2400 Ft/óra*</t>
+          <t>Br. 2536 Ft/óra</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1748,17 +1768,17 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.29122261232887436</t>
+          <t>ml_score=4, ml_prob=0.33348910664020065</t>
         </is>
       </c>
       <c r="J28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K28" t="n">
-        <v>0.2912226123288744</v>
+        <v>0.3334891066402006</v>
       </c>
       <c r="L28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1769,32 +1789,28 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>IT Support Specialist Trainee</t>
+          <t>IT biztonsági tanácsadó</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/it-support-specialist-trainee-budapest-3-ker--28030</t>
+          <t>https://muisz.hu/diakmunkaink/IT%20biztons%C3%A1gi%20tan%C3%A1csad%C3%B3%20-budapest-i-kerulet--21926</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>IT Support Specialist Trainee Graphisoft® empowers teams to design great buildings through award-winning software solutions, learning programs, and professional services for the AEC industry. Our award-winning products and solutions support OPEN BIM for workflow transparency, longevity, and data accessibility for built assets.  Archicad®, the architects’ BIM software of choice, offers a complete end-to-end design and documentation workflow for architectural and integrated architectural and engineering practices of any size. BIMx®, the most popular mobile and web BIM app, extends the BIM experience to include all stakeholders in the building design, delivery, and operations lifecycle. BIMcloud®, the AEC industry’s first and most advanced cloud-based team collaboration solution, makes real-time collaboration possible across the globe regardless of the size of the project and the speed or quality of the team members’ network connection. DDScad solutions support users with intelligent Mechanical, Electrical, and Plumbing (MEP) design tools, integrated calculations, and comprehensive documentation of all building system disciplines. Graphisoft is part of the Nemetschek Group. To learn more, visit more visit www.graphisoft.com Feladatok •	Provide on-site support in the Budapest office and assist with basic remote support for colleagues worldwide, in both English and Hungarian. •	Assist in end-user support for PCs, Macs, mobile devices (iOS and Android), printers, scanners, and video conferencing systems. •	Support colleagues in the effective use of collaboration platforms such as Microsoft Teams, SharePoint Online, and Miro. •	Participate in basic system administration tasks (Active Directory, Microsoft 365) under the guidance of senior team members. •	Provide first-level application support for Microsoft Teams, Outlook, Word, Excel, and PowerPoint. •	Help with incident and service request ticket handling: categorization, documentation, and updating users on progress. •	Contribute to maintaining user guides, FAQs, and process documentation. •	Assist with hardware asset tracking and lifecycle processes. •	Participate in basic network troubleshooting (DNS, DHCP, IP) with guidance from experienced colleagues. •	Gain exposure to emerging technologies and contribute ideas for improvements. Elvárások •	Ongoing studies in IT field at a Hungarian university. •	Active student status for at least 2 semesters. •	Proficiency in both English and Hungarian. •	Eagerness to learn and openness to new technologies. •	Customer-oriented mindset and willingness to respond quickly to requests. •	A minimum of 20 hours of work per week. •	Team player with a proactive and problem-solving attitude. •	Motivation to help others and build practical IT skills. Egyéb •	International, inspiring, and dynamic environment. •	Challenging and various tasks. •	Continuous learning &amp; development opportunities. •	The flexibility of a hybrid workplace with at least 1 day / week home office (after the probationary period). If you think this description fits you, come and join us in our company headquarters located at the well-known Graphisoft Park!</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>magyar</t>
-        </is>
-      </c>
+          <t>IT biztonsági tanácsadó Partnerünk több mint 10 éve kínál informatikai megoldásokat ügyfelei részére. Saját és ügyfeleik informatikai eszközeinek üzemeltetésére keresünk munkatársat az alábbi pozícióba: Junior IT biztonsági tanácsadó Feladatok •	Információbiztonsági kockázatok feltárása, elemzése, és javaslattétel a kezelésükre •	Információbiztonsági események azonosítása, felderítése, kivizsgálása és ezek alapján kockázatkezelésen alapuló tevékenységek meghatározása •	Informatikabiztonsági oktatás, tanácsadási munkákban való részvétel •	Információbiztonsági, adatkezelési szabályzatok elkészítése •	Információbiztonsági és GDPR auditok, felmérések támogatása ügyfeleinknél •	Információbiztonsági incidensek kivizsgálása •	Információbiztonsági eseményekhez, incidensekhez kapcsolódó napi jelentések, elemzések és beszámolók készítése Elvárások •	 Utolsó éves, felsőfokú információbiztonsági szakirányú műszaki vagy gazdaságinformatikai végzettség •	Hasonló munkakörben szerzett gyakorlat előny, de nem feltétel •	Irodai alkalmazások ismerete – MS Office, Outlook, böngészők •	Kitartó, önálló munkavégzés •	Analitikus és megoldásközpontú szemlélet, problémaorientált gondolkodás •	Precizitás, megbízhatóság •	Dinamikus, energikus munkavégzés Egyéb Amit kínálunk: •	Stabil háttér •	Szakmai kihívást jelentő, változatos feladatok •	Fiatalos, lendületes, együttműködő csapat •	Színvonalas irodai munkakörnyezet •	Családias légkör</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Budapest 3. ker.</t>
+          <t>Budapest 1. ker.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2005 Ft/ óra</t>
+          <t>2400 Ft/ óra</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1802,14 +1818,14 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.23130507951893228</t>
+          <t>ml_score=3, ml_prob=0.2584544944215462</t>
         </is>
       </c>
       <c r="J29" t="n">
         <v>3</v>
       </c>
       <c r="K29" t="n">
-        <v>0.2313050795189323</v>
+        <v>0.2584544944215462</v>
       </c>
       <c r="L29" t="n">
         <v>3</v>
@@ -1823,17 +1839,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Programozás oktatása (XI. kerület)</t>
+          <t>Informatikus gyakornok</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/programozas-oktatasa-xi-kerulet-budapest-xi-kerulet--12147</t>
+          <t>https://muisz.hu/diakmunkaink/informatikus-gyakornok-budaors--27645</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Programozás oktatása (XI. kerület) Jelentkezz nálunk egy érdekes és izgalmas munkára! LOGISCOOL BUDA-ÚJBUDA Programozás speciális, élmény alapú tanítására keresünk egyetemistákat, 16 év feletti középiskolásokat. Feladatok Iskolánk a Logiscool Buda-Újbuda, ( a központ cím: 1116 Budapest, Fehérvári út 108-112, és 1122 Budapest, Maros utca 12.) A tanítás 2025 szeptemberében kezdődik és folyamatosan tart az iskolai tanévekhez igazodva budai és újbudai területeken. Rugalmasan választható, órarendhez igazíthatóan tudsz nálunk csoportokat vállalni. Óráinkat a központi iskolánkban minden hétköznap délutánonként 14:00 - 18:30 óra között, valamint szombaton délelőtt tartjuk a 1,5-1,5 órás foglalkozásokat.  A kihelyezett helyszíneken budán és újbudán is hétköznapokon akár 13:00 tól is már kezdődnek foglalkozásaink. Rugalmasan lehetőséged van egy vagy több napot hetente, vagy 1 vagy több csoportot naponta kiválasztani a tanításra – bármelyiket, amelyik Neked megfelel. Előzetesen oktatóinknak tréninget tartunk. Elvárások Ha •	nyitott vagy gyerekek oktatására, esetleg tanítási tapasztalataid vannak, •	kiváló kommunikációs készséggel rendelkezel és jó előadó vagy, •	kedveled a gyerekeket és szót is tudsz érteni velük, •	informatikai, programozói ismeretekkel rendelkezel, (előny, de nem feltétel) •	jó megjelenésű, határozott fellépésű, érdekes személyiség vagy, aki példaképül is szolgálhat, •	a kreativitás nem áll messze tőled, •	megbízható és pontos vagy, •	ismered az angol nyelvet, akkor várunk, jelentkezz nálunk! Egyéb Megfelelő díjazást: nettó 2.000 – 2.500 Ft órabér, (minimum 2000.-Ft + bónusz az elvégzett feladatok teljesítménye alapján), hosszú távú lehetőséget, rugalmas, órarendhez igazítható kellemes munkakörülményeket kínálunk egy fiatal csapatban. Kölcsönös elégedettség esetén dolgozhatsz nálunk majd nyári táborainkban is!</t>
+          <t>Informatikus gyakornok CSATLAKOZZ TE IS A 20 ÉVES ALFAPED KFT CSAPATÁHOZ! Mindig is érdekelt, hogyan működik egy cég informatikai háttere? Szeretsz rendszerekben gondolkodni, prob-lémákat megoldani és új megoldásokat kipróbálni? Szívesen támogatnád mérnöki és projektcsapatainkat in-formatikai tudásoddal? Szeretnél egy fiatalos és jókedvű csapatban dolgozni? Akkor Te vagy a mi emberünk! INFORMATIKUS GYAKORNOKOT Rólunk: Az AlfaPed Kft. az energetikai tanácsadás és auditálás területén működő, dinamikusan fejlődő vállalat. Hiszünk abban, hogy a fenntarthatóság és az energiahatékonyság a jövő kulcsa. Cégünk 2005 óta van jelen a hazai energetikai tanácsadói piacon. Az alapítás óta eltelt több, mint 20 év alatt megőriztük a szakmai munkába vetett hitünket és a túlzott növekedés helyett inkább egy szakértőkből álló mérnöki munkaközösséget építettünk. Tettük ezt azért, hogy az energetikai felülvizsgálatok, auditok teljes spektrumát le tudjuk fedni. Az elmúlt időszakban számos multinacionális cégnél, illetve középvállaltnál végez-tünk energetikai veszteségfeltáró munkát és az általunk készített felméréseinkkel, audit jelentésekkel és tanul-mányokkal, igyekeztünk megalapozni az energetikai fejlesztések irányát. Munkánkra jellemző a komplexitás és a rendszerszemlélet, de ha az ügyféligény azt kívánja, akkor speciális feladatokban is elmélyedünk. Irodánk családias környezetben Budaörsön működik, ami autóval és tömegközlekedéssel egyaránt könnyen megközelíthető. (Kelenföldről 10-15 perc.) Fiatalos, támogató csapatunkban a szakmai fejlődés mellett olyan közösségre találsz, ahol számít a jókedv, a kölcsönös tisztelet és a bizalom. Feladatok Milyen feladatok várnak Rád? Építsd és fejleszd Önmagadat és szerezz minél gyorsabban és minél több tapasztalatot a kollégáink, és a kép-zési rendszerünk segítségével. (Cél: Dolgozd be magadat nálunk és amire végzel, lesz főállásod nálunk!) •	Fejleszthetsz Microsoft BI riportokat és dashboardokat •	Részt vehetsz AI eszközök tesztelésében és bevezetésében •	Foglalkozhatsz Power Platform fejlesztésekkel •	Segíthetsz az IT támogató eszközök üzemeltetésében és testreszabásában •	Belekóstolhatsz az energetikai veszteségfeltárás világába és az energetikai adatelemzésbe Elvárások Milyen szakmai ismeretek szükségesek? Nekünk Te számítasz és a fejlődni akarásod! Gyakornok pozícióról van szó, így nem várunk el 10 év szakmai ta-pasztalatot. •	Folyamatban lévő felsőfokú tanulmányok (Informatikus, IT biztonság, vagy automatizálás) •	Felhasználói szintű MS Office ismeret (Excel, Word, PowerPoint) •	Magabiztos kommunikáció magyar nyelven – angol nyelv előny Előnyt jelent: •	Programozói vagy programtervezői tapasztalat •	IT üzemeltetési tapasztalat •	Diák- vagy szakmai szervezetben végzett tevékenység •	TDK munka vagy tanszéki munkavégzés •	Kiemelkedő sport tevékenység, vagy bármilyen versenyeredmény Milyen személyiséget keresünk? Téged keresünk, amennyiben a következőkben magadra ismersz. •	Korrekt és megbízható vagy. Hosszútávú együttműködést keresel, nem csak alkalmi munkát. •	Jó a problémamegoldó készséggel és „can-do” attitűddel állsz hozzá a feladatokhoz. •	Rendszerszemlélettel rendelkezel, és a munkádra igényes vagy. •	Szereted az innovatív technológiákat megismerni és használni is. •	Nemcsak a problémákat látod, hanem a megoldásra is van javaslatod. Egyéb Mit biztosítunk? •	Induló bér: nettó 1.900 Ft/óra •	Akár 2 havi bónusz (év közi belépés esetén arányosított) •	Teljesítményalapú plusz jutalmak •	Egyéni fejlődéshez kötött grade rendszer. (A béremelés időpontja csak tőled függ!) •	Látható és kihirdetett karrier út: Gyakornok → Senior energetikus •	Rugalmas munkaidő és home office lehetőség •	Egyéni oktatási keret (gyakornokoknak is) •	Céges képzések, és konferenciák (az egyéni oktatási kereten felül) •	Kötelező szakmai gyakorlat igazolása (fizetett keretek között) •	Diplomamunka írás lehetősége és mentorálás •	Hosszútávú munkalehetőség •	Családias és fiatalos munkakörnyezet •	Céges autó használat („kulcsos autó” - privát célra is) •	Notebook és céges mobiltelefon Hogyan tudsz jelentkezni? Amennyiben szívesen csatlakoznál hozzánk, az alábbi módon tudsz jelentkezni: 1. Írj egy saját motivációs levelet vagy válaszold meg a következő kérdéseket néhány mondatban! •	Miért érdekel Téged az informatika és az adatelemzés? •	Milyen tapasztalattal rendelkezel automatizálás és adatelemzési területeken? •	Mit szeretnél megtanulni nálunk? •	Mely eredményedre voltál a legbüszkébb az életedben? •	Mi az a legfontosabb dolog, amit a szüleidtől tanultál? •	Milyen egy jó csapat szerinted? •	Te ehhez mit tudnál hozzá adni, ha csak 1 dolgot lehetne mondani? •	Miért Te a legalkalmas erre a pozícióra? Mit üzensz a jövőbeli kollégáidnak?</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1844,7 +1860,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2000-2500 Ft/ óra</t>
+          <t>2200 Ft/ óra + bónuszok</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -1852,71 +1868,71 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.26474386097465424</t>
+          <t>ml_score=5, ml_prob=0.4172016627488708</t>
         </is>
       </c>
       <c r="J30" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K30" t="n">
-        <v>0.2647438609746542</v>
+        <v>0.4172016627488708</v>
       </c>
       <c r="L30" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>schonherz</t>
+          <t>muisz</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Full-stack fejlesztő</t>
+          <t>C++ programozó</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40774-full-stack-fejleszto</t>
+          <t>https://muisz.hu/diakmunkaink/c-programozo-budapest-iii-kerulet--25576</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>🏢 Partnerünk Magyarország egyik legmodernebb vendéglátó szoftverének fejlesztő cége. Céljuk nemcsak az, hogy rendszerük egyszerűen használható, gyors és megbízható legyen, hanem az is, hogy minden kapcsolódó szolgáltatásuk kimagasló színvonalat képviseljen. Mindezzel felfrissítve és megreformálva a vendéglátás területét. Feladatok: 🎮 Termékfejlesztés, bekapcsolódás a tervezésbe 🎮 Új funkciók fejlesztése 🎮 Meglévő funkciók továbbfejlesztése, kiegészítése 🎮 Új technológiák kipróbálása, beépítése a fejlesztési folyamatba 🎮 Visszajelzések kezelése, problémák megoldása, hibajavítás 🎮 Fejlesztői csapat munkájának támogatása 🎮 Aktív részvétel a projektekben és a szoftverek minőségének folyamatos javításában Elvárások: 🧩 Informatikai felsőoktatását elvégezte már 🧩 Minimum 1-2 év munkatapasztalat 🧩 Dolgozott munkahelyén már Spring Boot és React stack technológiákkal. 🧩 Önéletrajz a korábbi tapasztalatok részletes megjelölésével 🧩 Minimum középfokon beszél angolul. 🧩 Verziókezelő szoftverek ismerete (pl: Git) 🧩 Java, Javascipt programozási nyelv ismerete és gyakorlat a használatában 🧩 Kódolási szabványok és best practice-ek követése 🧩 Igényes a kódjára és szeret megoldani, nem csak “megcsinálni” 🧩 Hozzáállásában proaktív, megoldásközpontú 🧩 Erős problémamegoldó gondolkodás (hibakeresés, root cause, kreatív megoldások) 🧩 Rendszerszintű szemlélet 🧩 Önállóság és ownership (feladat végigvitele, felelősségvállalás) 🧩 Csapatban való jó együttműködés (code review, közös döntések) 🧩 Nyitottság a tanulásra és a fejlődésre ⏰ Munkaidő: 09:00 - 17:00. Nincs home office. ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+          <t>C++ programozó Professzionális 3D CAD / BIM tervezőszoftver fejlesztésével foglalkozó partnercégünk keres fejlesztő, programozó diákokat. Feladatok -Csővezeték méretezés algoritmus Elvárások -Áramlástani ismeretek -C++ vagy C# 1-2 éves tapasztalat</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Angol középfok</t>
+          <t>magyar, angol</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Budapest XIII. kerület</t>
+          <t>Budapest 3. ker.</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Megegyezés szerint</t>
+          <t>2500 Ft/óra</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>ml_score=4, ml_prob=0.37450018125204043</t>
+          <t>ml_score=3, ml_prob=0.24219736063802752</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K31" t="n">
-        <v>0.3745001812520404</v>
+        <v>0.2421973606380275</v>
       </c>
       <c r="L31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -1927,32 +1943,32 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Frontend fejlesztő</t>
+          <t>Szoftverfejlesztő</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40729-frontend-fejleszto</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40776-szoftverfejleszto</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>🏢 Partnerünk átfogó szoftverfejlesztéssel foglalkozik, egészen a tervezéstől a karbantartásig. Felhőalapú megoldásaikkal hatékonyabbá, biztonságosabbá és fenntarthatóbbá teszik a vállalkozásokat. Feladatok: 🧩 Fejlesztési feladatok: 📝 Webes/cross-platform applikációk fejlesztése főként vállalati portálokhoz, oktatási rendszerekhez a legújabb technológiákban (Vue, React, React Native) 📝 Cloud architechtúra alapú fejlesztések 📝 Friss, gyors átfutási idővel (3-6 hónap / projekt) rendelkező projektek 📝 Rugalmasan oszthatod be a munkaóráid 🧩Adminisztratív teendőkhöz: 📝 GitLab-en rögzített teendőid áttekintése, elvégzése 📝 Kérdések esetén egyeztetés, könnyen, gyorsan, Teams-en Elvárások: 🎯 Folyamatban lévő felsőfokú tanulmányok 🎯 Vue.js ÉS React ismeret 🎯 Az önéletrajz kézhezvételét követően próbafeladat megoldása szükséges 🎯 Angol társalgási szintű nyelvtudás 🎯 Informatikai beállítottság, pontosság Munkakörnyezet: 🏢 Home Office lehetőség 🏢 Igény esetén a III. kerületi irodában is biztosított a munkavégzés (nem kötelező) ⏰ Munkaidő: Kötetlen ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami 693 700 Ft havonta.</t>
+          <t>Partnerünk egy információszolgáltatással foglalkozó technológiai vállalat, amely az üzleti technológiákra specializálódik. Rendszerintegrációval, tanácsadással és szoftverfejlesztéssel nyújtanak IT-szolgáltatásokat. A szerver-, hálózati-, egységes kommunikációs technológiák és a szoftverfejlesztés területén szerzett mély szakértelmünkkel segítünk vállalkozásodnak növekedni és fejlődni a kitűzött célokkal összhangban. Hiszünk abban, hogy egyszerre tehetjük vállalkozásodat egyszerűbbé és hatékonyabbá. 💼 Egyszerre több projekt van folyamatban. A projekteken a kollégák csapatban dolgoznak, és egy vezető fejlesztő koordinálja a munkát. 🎯 Figyelembe veszik, hogy kinek mi az erőssége, illetve mely területek érdeklik jobban, és ennek megfelelően osztják le a feladatokat. 🌱 Többnyire univerzális munkatársakat keresnek, akik nyitottak a fejlődésre és tanulásra, és a preferált programozási területükön kívül más területeken is rendelkeznek alapszintű tudással. 🧭 A belépést követően egy tesztfeladatsoron kell végigmenni, amely pár hétig tart. Ez idő alatt megismerik a cég főbb szakmai irányvonalait, és egy kijelölt mentor segíti őket. Feladatok: ⬛️ Szoftverfejlesztés ⬛️ Részvétel az üzemeltetési feladatokban 💻 Használt backend technológiák: Java Quarkus, Java Spring, NodeJS Használt frontend technológiák: VueJS, Angular. Nem baj, ha nem ismered mindet, de légy nyitott más programnyelvek elsajátítására is. Elvárások: ✔️ Folyamatban lévő felsőfokú tanulmányok, lehetőleg végzéshez közel ✔️ Linux alapismeretek ✔️ Java programozási nyelv magabiztos ismerete ✔️ 3 félév elvégzése a megfelelő felsőoktatási programban vagy szakmai tapasztalat ✔️ Angol aktív szövegértés/szóbeli kommunikáció, írásban kevésbé használatos ✔️ Heti minimum 32 óra várható munkavégzés ✔️ Munkatapasztalat megjelölése, leírása ✔️ Referencia munka-link küldése ✔️ Motivációs levél ✔️ Legyen MySQL és minimális hálózati ismereted ✔️ Partnerrel történő találkozás során elegáns, hivatalos megjelenés ✔️ Önálló munkavégzésre való törekvés ✔️ Megbízhatóság ✔️ Csapatmunka ✔️ Precizitás ✔️ Pontosság ✔️ Határidők betartása ✔️ Jogosítvány nem feltétel, de megléte esetén a későbbiekben cégautó használat lehetősége fennáll Amit Partnerünk kínál: 🏡 14. kerületi családias lakásiroda, bogrács és medence is a rendelkezésre áll. 🇭🇺 Magyar tulajdonban lévő vállalkozás. 👨‍💻 Az Ügyvezető, egyben tulajdonos IT területről érkezett, részt vesz folyamatosan a projektekben. 🅿️ Utcán a parkolás ingyenes 🌳 Zugló kertvárosi részén, 3 emeletes villa kerttel, medencével 🎯 A pince klubhelyiséggé lett kialakítva (csocsó, pingpong, darts) 🤝 Családias hangulat, kb. 20 fő alkalmazott 🧑‍🎓 Átlag életkor 30 év alatti, egyetem mellett dolgozó, egyetemet végző, friss diplomás kollégák, szoftverfejlesztők 🎉 Rendszeres csapatépítők, bográcsozás, vetélkedős estek. Az irodában kávé, tea, víz, sós és édes és egyéb szezonnak megfelelő nassolnivalók a rendelkezésre állnak Hosszútávú munkalehetőség, a tanulmányok után főállású pozíció is elnyerhető. 📚 Nem csak a szakmai gyakorlatod leigazolásában, de akár a szakdolgozatodban is szívesen segítünk. 📅 Munkaidő: Kötetlen munkarend ⏰ Törzsidő : 9:00-16:00 Alapvetően irodai munkavégzés, az első 3-6 hónapban biztosan bejárós, de ha önállóan tudsz dolgozni, akkor 1-2 nap HO is oké a későbbiekben. ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Angol társalgási szint</t>
+          <t>Angol (Középfok)</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Home office</t>
+          <t>Budapest XIV. kerület</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Br. 2536 Ft/óra</t>
+          <t>Br. 2200-2400 Ft/óra*</t>
         </is>
       </c>
       <c r="H32" t="n">
@@ -1960,99 +1976,107 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>ml_score=4, ml_prob=0.33348910664020065</t>
+          <t>ml_score=3, ml_prob=0.29122261232887436</t>
         </is>
       </c>
       <c r="J32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K32" t="n">
-        <v>0.3334891066402006</v>
+        <v>0.2912226123288744</v>
       </c>
       <c r="L32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>muisz</t>
+          <t>schonherz</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>IT biztonsági tanácsadó</t>
+          <t>Full-stack fejlesztő</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/IT%20biztons%C3%A1gi%20tan%C3%A1csad%C3%B3%20-budapest-i-kerulet--21926</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40774-full-stack-fejleszto</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>IT biztonsági tanácsadó Partnerünk több mint 10 éve kínál informatikai megoldásokat ügyfelei részére. Saját és ügyfeleik informatikai eszközeinek üzemeltetésére keresünk munkatársat az alábbi pozícióba: Junior IT biztonsági tanácsadó Feladatok •	Információbiztonsági kockázatok feltárása, elemzése, és javaslattétel a kezelésükre •	Információbiztonsági események azonosítása, felderítése, kivizsgálása és ezek alapján kockázatkezelésen alapuló tevékenységek meghatározása •	Informatikabiztonsági oktatás, tanácsadási munkákban való részvétel •	Információbiztonsági, adatkezelési szabályzatok elkészítése •	Információbiztonsági és GDPR auditok, felmérések támogatása ügyfeleinknél •	Információbiztonsági incidensek kivizsgálása •	Információbiztonsági eseményekhez, incidensekhez kapcsolódó napi jelentések, elemzések és beszámolók készítése Elvárások •	 Utolsó éves, felsőfokú információbiztonsági szakirányú műszaki vagy gazdaságinformatikai végzettség •	Hasonló munkakörben szerzett gyakorlat előny, de nem feltétel •	Irodai alkalmazások ismerete – MS Office, Outlook, böngészők •	Kitartó, önálló munkavégzés •	Analitikus és megoldásközpontú szemlélet, problémaorientált gondolkodás •	Precizitás, megbízhatóság •	Dinamikus, energikus munkavégzés Egyéb Amit kínálunk: •	Stabil háttér •	Szakmai kihívást jelentő, változatos feladatok •	Fiatalos, lendületes, együttműködő csapat •	Színvonalas irodai munkakörnyezet •	Családias légkör</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>🏢 Partnerünk Magyarország egyik legmodernebb vendéglátó szoftverének fejlesztő cége. Céljuk nemcsak az, hogy rendszerük egyszerűen használható, gyors és megbízható legyen, hanem az is, hogy minden kapcsolódó szolgáltatásuk kimagasló színvonalat képviseljen. Mindezzel felfrissítve és megreformálva a vendéglátás területét. Feladatok: 🎮 Termékfejlesztés, bekapcsolódás a tervezésbe 🎮 Új funkciók fejlesztése 🎮 Meglévő funkciók továbbfejlesztése, kiegészítése 🎮 Új technológiák kipróbálása, beépítése a fejlesztési folyamatba 🎮 Visszajelzések kezelése, problémák megoldása, hibajavítás 🎮 Fejlesztői csapat munkájának támogatása 🎮 Aktív részvétel a projektekben és a szoftverek minőségének folyamatos javításában Elvárások: 🧩 Informatikai felsőoktatását elvégezte már 🧩 Minimum 1-2 év munkatapasztalat 🧩 Dolgozott munkahelyén már Spring Boot és React stack technológiákkal. 🧩 Önéletrajz a korábbi tapasztalatok részletes megjelölésével 🧩 Minimum középfokon beszél angolul. 🧩 Verziókezelő szoftverek ismerete (pl: Git) 🧩 Java, Javascipt programozási nyelv ismerete és gyakorlat a használatában 🧩 Kódolási szabványok és best practice-ek követése 🧩 Igényes a kódjára és szeret megoldani, nem csak “megcsinálni” 🧩 Hozzáállásában proaktív, megoldásközpontú 🧩 Erős problémamegoldó gondolkodás (hibakeresés, root cause, kreatív megoldások) 🧩 Rendszerszintű szemlélet 🧩 Önállóság és ownership (feladat végigvitele, felelősségvállalás) 🧩 Csapatban való jó együttműködés (code review, közös döntések) 🧩 Nyitottság a tanulásra és a fejlődésre ⏰ Munkaidő: 09:00 - 17:00. Nincs home office. ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Angol középfok</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Budapest 1. ker.</t>
+          <t>Budapest XIII. kerület</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2400 Ft/ óra</t>
+          <t>Megegyezés szerint</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.2584544944215462</t>
+          <t>ml_score=4, ml_prob=0.37450018125204043</t>
         </is>
       </c>
       <c r="J33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K33" t="n">
-        <v>0.2584544944215462</v>
+        <v>0.3745001812520404</v>
       </c>
       <c r="L33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>muisz</t>
+          <t>schonherz</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Informatikus gyakornok</t>
+          <t>Machine Learning Engineer Intern</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/informatikus-gyakornok-budaors--27645</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40713-machine-learning-engineer-intern</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Informatikus gyakornok CSATLAKOZZ TE IS A 20 ÉVES ALFAPED KFT CSAPATÁHOZ! Mindig is érdekelt, hogyan működik egy cég informatikai háttere? Szeretsz rendszerekben gondolkodni, prob-lémákat megoldani és új megoldásokat kipróbálni? Szívesen támogatnád mérnöki és projektcsapatainkat in-formatikai tudásoddal? Szeretnél egy fiatalos és jókedvű csapatban dolgozni? Akkor Te vagy a mi emberünk! INFORMATIKUS GYAKORNOKOT Rólunk: Az AlfaPed Kft. az energetikai tanácsadás és auditálás területén működő, dinamikusan fejlődő vállalat. Hiszünk abban, hogy a fenntarthatóság és az energiahatékonyság a jövő kulcsa. Cégünk 2005 óta van jelen a hazai energetikai tanácsadói piacon. Az alapítás óta eltelt több, mint 20 év alatt megőriztük a szakmai munkába vetett hitünket és a túlzott növekedés helyett inkább egy szakértőkből álló mérnöki munkaközösséget építettünk. Tettük ezt azért, hogy az energetikai felülvizsgálatok, auditok teljes spektrumát le tudjuk fedni. Az elmúlt időszakban számos multinacionális cégnél, illetve középvállaltnál végez-tünk energetikai veszteségfeltáró munkát és az általunk készített felméréseinkkel, audit jelentésekkel és tanul-mányokkal, igyekeztünk megalapozni az energetikai fejlesztések irányát. Munkánkra jellemző a komplexitás és a rendszerszemlélet, de ha az ügyféligény azt kívánja, akkor speciális feladatokban is elmélyedünk. Irodánk családias környezetben Budaörsön működik, ami autóval és tömegközlekedéssel egyaránt könnyen megközelíthető. (Kelenföldről 10-15 perc.) Fiatalos, támogató csapatunkban a szakmai fejlődés mellett olyan közösségre találsz, ahol számít a jókedv, a kölcsönös tisztelet és a bizalom. Feladatok Milyen feladatok várnak Rád? Építsd és fejleszd Önmagadat és szerezz minél gyorsabban és minél több tapasztalatot a kollégáink, és a kép-zési rendszerünk segítségével. (Cél: Dolgozd be magadat nálunk és amire végzel, lesz főállásod nálunk!) •	Fejleszthetsz Microsoft BI riportokat és dashboardokat •	Részt vehetsz AI eszközök tesztelésében és bevezetésében •	Foglalkozhatsz Power Platform fejlesztésekkel •	Segíthetsz az IT támogató eszközök üzemeltetésében és testreszabásában •	Belekóstolhatsz az energetikai veszteségfeltárás világába és az energetikai adatelemzésbe Elvárások Milyen szakmai ismeretek szükségesek? Nekünk Te számítasz és a fejlődni akarásod! Gyakornok pozícióról van szó, így nem várunk el 10 év szakmai ta-pasztalatot. •	Folyamatban lévő felsőfokú tanulmányok (Informatikus, IT biztonság, vagy automatizálás) •	Felhasználói szintű MS Office ismeret (Excel, Word, PowerPoint) •	Magabiztos kommunikáció magyar nyelven – angol nyelv előny Előnyt jelent: •	Programozói vagy programtervezői tapasztalat •	IT üzemeltetési tapasztalat •	Diák- vagy szakmai szervezetben végzett tevékenység •	TDK munka vagy tanszéki munkavégzés •	Kiemelkedő sport tevékenység, vagy bármilyen versenyeredmény Milyen személyiséget keresünk? Téged keresünk, amennyiben a következőkben magadra ismersz. •	Korrekt és megbízható vagy. Hosszútávú együttműködést keresel, nem csak alkalmi munkát. •	Jó a problémamegoldó készséggel és „can-do” attitűddel állsz hozzá a feladatokhoz. •	Rendszerszemlélettel rendelkezel, és a munkádra igényes vagy. •	Szereted az innovatív technológiákat megismerni és használni is. •	Nemcsak a problémákat látod, hanem a megoldásra is van javaslatod. Egyéb Mit biztosítunk? •	Induló bér: nettó 1.900 Ft/óra •	Akár 2 havi bónusz (év közi belépés esetén arányosított) •	Teljesítményalapú plusz jutalmak •	Egyéni fejlődéshez kötött grade rendszer. (A béremelés időpontja csak tőled függ!) •	Látható és kihirdetett karrier út: Gyakornok → Senior energetikus •	Rugalmas munkaidő és home office lehetőség •	Egyéni oktatási keret (gyakornokoknak is) •	Céges képzések, és konferenciák (az egyéni oktatási kereten felül) •	Kötelező szakmai gyakorlat igazolása (fizetett keretek között) •	Diplomamunka írás lehetősége és mentorálás •	Hosszútávú munkalehetőség •	Családias és fiatalos munkakörnyezet •	Céges autó használat („kulcsos autó” - privát célra is) •	Notebook és céges mobiltelefon Hogyan tudsz jelentkezni? Amennyiben szívesen csatlakoznál hozzánk, az alábbi módon tudsz jelentkezni: 1. Írj egy saját motivációs levelet vagy válaszold meg a következő kérdéseket néhány mondatban! •	Miért érdekel Téged az informatika és az adatelemzés? •	Milyen tapasztalattal rendelkezel automatizálás és adatelemzési területeken? •	Mit szeretnél megtanulni nálunk? •	Mely eredményedre voltál a legbüszkébb az életedben? •	Mi az a legfontosabb dolog, amit a szüleidtől tanultál? •	Milyen egy jó csapat szerinted? •	Te ehhez mit tudnál hozzá adni, ha csak 1 dolgot lehetne mondani? •	Miért Te a legalkalmas erre a pozícióra? Mit üzensz a jövőbeli kollégáidnak?</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>📍Our Partner provides a platform that supports requirements engineering, development, and testing in both Agile and V-model processes. It enhances productivity and quality by enabling knowledge reuse, semantic search, and the detection of duplicates, similarities, and inconsistencies, as well as offering contextual and domain-specific authoring support. The platform integrates seamlessly with a wide range of software engineering tools, ensuring compatibility and ease of use, and can be deployed on-premise or as a SaaS solution. 🤖 The company is looking for a highly motivated Machine Learning Intern to join its dynamic team. In this role, the intern will support the AI team in their daily operations. Responsibilities: 🧠 Assist in the design, development, and deployment of machine learning models 📊 Work with large datasets, including data preprocessing, feature engineering, and analysis 🤝 Collaborate with the team to improve the accuracy and performance of machine learning models ⚙️ Maintain automated pipelines for model training, testing, and evaluation Requirements: 🎓 Ongoing Bachelor’s or Master’s studies (a must) 📘 Preferred fields: Computer Engineering, Software Engineering, Bioinformatics, Electrical Engineering, or potentially Finance 🤖 Strong interest and/or experience in: • LLM fine-tuning • Retrieval-Augmented Generation (RAG) • Machine Learning / Deep Learning • NLP / GenAI • Computer Vision / Object Detection 🐍 Practical experience with Python and PyTorch 🗣️ Language skills: 🇨🇳 Fluent Chinese (native or advanced) 🇬🇧 English at B2 level or higher ❗ Hungarian is not required 🤝 Ability to work collaboratively across teams 📌 Capable of managing multiple priorities effectively 🌟 Enjoys working in a highly skilled, competitive team with flat hierarchies 🎁 What our Partner offers: 🌍 Flexible working location and flexible working hours 🤝 Strong team spirit, with a mentor/buddy program to support your onboarding 🏆 Access to world-class clients and a cutting-edge product shaping the next industrial revolution 💰 Competitive remuneration 🎉 Regular offsite team-building events 🏢 Modern office located at Deák Ferenc tér 🕘 Working arrangement: flexible, primarily remote work, with approximately one day per month required in the office ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Send us your english CV with a photo to the hr@schonherz.hu e-mail adress! * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 693,700 per month.</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>English and Chinese (fluent)</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Budapest 11. ker.</t>
+          <t>Home office</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2200 Ft/ óra + bónuszok</t>
+          <t>Gross 3000 Ft/hour*</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -2060,53 +2084,53 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>ml_score=5, ml_prob=0.4172016627488708</t>
+          <t>ml_score=3, ml_prob=0.2658357664748733</t>
         </is>
       </c>
       <c r="J34" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K34" t="n">
-        <v>0.4172016627488708</v>
+        <v>0.2658357664748733</v>
       </c>
       <c r="L34" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>muisz</t>
+          <t>schonherz</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>C++ programozó</t>
+          <t>Fejlesztőmérnök</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://muisz.hu/diakmunkaink/c-programozo-budapest-iii-kerulet--25576</t>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40636-fejlesztomernok</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>C++ programozó Professzionális 3D CAD / BIM tervezőszoftver fejlesztésével foglalkozó partnercégünk keres fejlesztő, programozó diákokat. Feladatok -Csővezeték méretezés algoritmus Elvárások -Áramlástani ismeretek -C++ vagy C# 1-2 éves tapasztalat</t>
+          <t>📐 Partnercégünk a csomagolástechnikában alkalmazott, nyomaték- és erőmérő műszerek gyártásának nemzetközileg elismert, exportorientált szereplője. Feladatok: 🎁 Egyedi nyomaték- és erőmérő rendszerek fejlesztése 🎁 Elektronikai és mechanikai komponensek integrálása 🎁 Gépek összeszerelése, tesztelése, kalibárlása 🎁 Szoftverfejlesztés és tesztelés (C++, PLC ladder logic) 🎁 (Mechatronikus esetén) 3D modellezés SolidWorks-ben Elvárások: ✅ Folyamatban lévő felsőfokú tanulmányok BME, esetleg Óbudai Egyetem, vagy hasonló egyetemeken ✅ Magas szintű C++ programozási ismeret ✅ PLC ladder logic ismerete ✅ Angol nyelvtudás legalább középszinten (műszaki dokumentáció szintjén) ✅ 3D modellezés tapasztalat SolidWorks-ben ✅ Precizitás, önállóság ✅ Jó problémamegoldó szemlélet Amit Partnerünk kínál: 🧩 Hosszú távú, stabil mérnöki munka kis csapatban, angol nyelvi környezetben 📍 Teljes vagy részmunkaidős foglalkoztatás 💎 Valódi termékfejlesztési tapasztalat, nem „összeszerelés” 💸 Versenyképes jövedelem ⏳ Rugalmas munkaidő 🎲 Szakmai fejlődési lehetőség 🖥️ Színvonalas munkakörnyezet ⏰ Munkaidő: általános irodai munkarend (kb. 08:00-17:00 között), Partner osztja be a diákkal rugalmasan egyeztetve ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami jelenleg 693 700 Ft havonta!</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>magyar, angol</t>
+          <t>Angol (Középfok)</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Budapest 3. ker.</t>
+          <t>Budapest, XXII. kerület</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2500 Ft/óra</t>
+          <t>Br. 4000 Ft/óra*</t>
         </is>
       </c>
       <c r="H35" t="n">
@@ -2114,16 +2138,432 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>ml_score=3, ml_prob=0.24219736063802752</t>
+          <t>ml_score=3, ml_prob=0.2915981866587006</t>
         </is>
       </c>
       <c r="J35" t="n">
         <v>3</v>
       </c>
       <c r="K35" t="n">
-        <v>0.2421973606380275</v>
+        <v>0.2915981866587006</v>
       </c>
       <c r="L35" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>schonherz</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Power Platform Gyakornok</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/39973-power-platform-gyakornok</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>💼 Partnerünk 2003-ban alakult, a munkatársak és vezetők tulajdonában álló, 120 fős vállalat stabil üzleti és pénzügyi háttérrel, több mint 50 visszatérő nagyvállalati ügyféllel. Üzleti problémák támogatására fejlesztenek ki és vezetnek be alkalmazásokat, valamint üzemeltetik azokat. Az üzleti folyamatautomatizáció a legerősebb megkülönböztető jegyük. ✅ A programjukban sok újdonságot fogsz megismerni. Teljes körű tag leszel az egyik csapatukban, ahol éles üzleti környezetben kapott feladatokon keresztül megtapasztalhatod, hogy milyen egy komplex, nagyvállalati projektben, szolgáltatásban dolgozni. 🌤️ A Program első hónapja a tanulásról szól online tananyagok és terület specifikus gyakorló feladatok segítségével. Ezután egy sikeres értékelő beszélgetést követően bekerülsz egy projekt csapatba, ahol már éles gyakorlati projektekben, szolgáltatásokban fejlesztheted tovább tudásodat, valós ügyfél feladatokat megoldva. Feladatok: 🌿 Projektcsapat tagjaként egyedi megoldások kialakítása a cég partnerei számára 🌿 Power Platform alapú low-code/no-code megoldások kialakítása a cég partnerei számára 🌿 Részvétel a kapcsolódó support tevékenységekben 🌿 Hibaanalízis és megoldási alternatívák kidolgozása 🌿 Esetenként üzleti követelményspecifikációk elemzése és az alkalmazás technikai elvárásainak megfogalmazása Elvárások: 🫐 Folyamatban lévő egyetemi vagy főiskolai tanulmányok aktív vagy passzív nappali tagozaton IT szakon 🫐 Informatikai megoldások iránti nyitottság, elsősorban megoldások tervezése, kialakítása fejlesztése 🫐 Power Platform vagy más no-code/low-code eszközök ismerete 🫐 Power apps vagy power automate tapasztalat 🫐 Alap programozási ismeretek, preferáltan TypeScript, JavaScript vagy C# nyelven React és SharePoint ismerete 🫐 Magabiztos angol nyelvtudás szóban és írásban egyaránt Amit a Partnerünk kínál: 📈 Rendszeres teljesítményértékelő/célkitűző beszélgetésen nézel rá a vezetőddel, merre tart a karriered és tudásod 🧙‍♂️ Egy dedikált mentor áll majd melletted, akihez mindig fordulhatsz és aki kíséri a szakmai utad 🌵 Versenyképes, mély szakmai tudásra tehetsz szert, amit valós projekteken, nagyvállalati ügyfelek üzleti kritikus rendszereivel dolgozva szerezhetsz meg 📍 Microsoft vizsgáid megszerzését támogatja Partnerünk 📙 Udemy kurzusokon keresztül tovább mélyítheted a tudásod 💡 Innovatív, inspiráló és barátságos környezetben dolgozhatsz ⏰ Munkaidő: Általános, heti 2 nap irodai munkavégzés, a többi Home Office-ból is lehet ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Angol (Középfok)</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Budapest, XI. kerület + Home Office</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Br. 2400 Ft/óra*</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>ml_score=4, ml_prob=0.39673552645675625</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>4</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.3967355264567562</v>
+      </c>
+      <c r="L36" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>muisz</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Test Engineer Trainee</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://muisz.hu/diakmunkaink/Test-engineer-trainee-xi-kerulet--28354</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Test Engineer Trainee “Today the community of around 1800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems and you can even find them/us in electric cars. There are hardly any industrial areas where the programs I and my colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members more than 30 years ago. As of today, our headcount has reached the 1800 employees and we are expanding – join us, be part of our team!” We are looking for a new colleague who will join our office in Budapest: Feladatok •	The Test Engineer trainee is responsible for the support of planning, execution and documentation of the Train IT tests, according to norms and specifications within the specified time frame. Main tasks: •	Preparation of the tests incl. test environment •	Execution of the tests according to the test instructions •	Analysis on any identified deviations from expected results and their possible causes •	Documentation of the tests carried out, the tests environment and the test conditions •	Testing mechanical hardware, electrical hardware and software Elvárások •	Testing methodology •	Analytical skills and solution-oriented •	Structured and systematic approach •	English knowledge Egyéb Not required but a plus: •	Python knowledge (target level: basic) •	Git and Svn •	Behaviour Driven Development approach What we offer: •	A young, dynamic, supporting team with mentor(s) •	Thesis topic and writing opportunity with an in-house consultant •	Home Office opportunity, flexible working hours •	Recreational opportunities within the office building (table football, table tennis) •	Free training opportunities •	Attractive working environment and secure workplace •	Free coffee and fruit days •	Various career options</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>magyar, angol</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Budapest 11. ker.</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2200-2800 Ft/óra</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>ml_score=3, ml_prob=0.20957823751535756</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>3</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.2095782375153576</v>
+      </c>
+      <c r="L37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>muisz</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>C++ developer trainee - UMC</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://muisz.hu/diakmunkaink/C%2B%2B%20developer-trainee-xi-kerulet--28355</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>C++ developer trainee - UMC “Today the community of around 1800 IT professionals and engineers believe – along with me – that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems and you can even find them/us in electric cars. There are hardly any industrial areas where the programs I and my colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members more than 30 years ago. As of today, our headcount has reached the 1800 employees and we are expanding – join us, be part of our team!” We are looking for a new colleague who will join our office in Budapest: Feladatok User Management Component (UMC) is used in many Siemens industry automation SW products to provide a unified interface for the end customer for user management and authentication. With the help of UMC, end customers are able to provision users/groups from MS Active Directory, use user management and authentication in distributed IT networks and federate to other Identity Providers. With UMC it is not only possible to support large factories but also make the life of smaller companies more secure. Tasks: •	Analyzing bugs coming from customers •	Supporting the development team in development, testing, and automation tasks •	Participating in the development of user management systems in C++ language, on Windows and Linux environments Elvárások •	Ongoing studies in a relevant field (informatics, programming) •	Knowledge in C++ programming •	Basic knowledge of Linux •	Ability to work independently and in a team •	Good English communication and negotiation skills •	Proactivity and willingness to learn, due to the complex developer environment Egyéb Advantages: •	Fluent in German •	Familiarity with version control tools such as TFS or GIT •	Experience in testing and test automation What we offer: •	Pleasant working environment in a youthful, dynamic team •	Opportunity for home office and flexible working hours •	International environment, stable and reliable background •	Various career opportunities</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>magyar, angol</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Budapest 11. ker.</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2200-2800 Ft/óra</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>ml_score=3, ml_prob=0.22574703382856207</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>3</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.2257470338285621</v>
+      </c>
+      <c r="L38" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>schonherz</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>AI Platform Operations Intern (AI &amp; Data Innovation Tribe)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40906-ai-platform-operations-intern-ai-data-innovation-tribe</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>⚡ Építs velünk AI platformot! Ha megy a Python és az SQL, és szívesen dolgoznál modern felhő alapú környezetben, jelentkezz Partnerünkhöz gyakornoknak! 🏢 Partnerünk a hazai távközlési piac teljes szolgáltatás-portfólióját elérhetővé teszi, legyen szó kommunikációs megoldásokról vagy szórakozásról. A cég tevékenysége révén három alapvető üzleti területet fed le: - vezetékes és mobilkommunikációs lakossági szolgáltatásokat - kis- és középvállalati szolgáltatásokat  - nagyvállalati ügyfeleknek nyújtott vállalati szolgáltatásokat. Feladatok: 🐍 Aktív részvétel az AI platform napi üzemeltetésében 🐍 A rendszerek elérhetőségének és stabilitásának biztosítása 🐍 Közreműködés Python alapú RESTful API-k fejlesztésében 🐍 API-k tesztelése és dokumentálása 🐍 A rendszerteljesítmény folyamatos figyelése és monitoringja 🐍 Naplófájlok elemzése és javaslattétel a hibák elhárítására 🐍 Ismerkedés a Google Cloud Platform (GCP) eszköztárával 🐍 Részvétel a felhő alapú infrastruktúra-kezelési feladatokban Elvárások: 🟢 Folyamatban lévő felsőfokú szakirányú tanulmányok (informatikai, mérnöki vagy matematikai területen) 🟢 Alapszintű, magabiztos tudás Python nyelven 🟢 Az SQL alapelveinek ismerete (lekérdezések, táblák kezelése) 🟢 Alapvető Linux/Unix parancssoros ismeretek 🟢 A Git verziókezelő használata 🟢 Nyitottság az új technológiák gyors elsajátítására 🟢 Proaktív attitűd a feladatokhoz Munkakörnyezet: 🚀 Valódi szakmai fejlődés: Partnerünk egyik legizgalmasabb AI platformjának építésében vehetsz részt 💡 Mentorálás: tapasztalt fejlesztőktől tanulhatod meg a modern szoftverfejlesztés és üzemeltetés (DevOps/MLOps) alapjait 🕒 Rugalmasság: a tanulás az első, így a munkaidőt az egyetemi óráidhoz igazítják 🏠 Modern környezet: Home Office lehetőség és inspiráló irodai légkör ⏰ Munkaidő: A feladatokat és a munkaidőt a Partner osztja be, a tanulmányok figyelembevételével. ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Budapest, IX. kerület + Home Office</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Br. 3000 Ft/óra*</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>ml_score=4, ml_prob=0.33744309409950285</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>4</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.3374430940995028</v>
+      </c>
+      <c r="L39" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>schonherz</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Data Analyst intern</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40905-data-analyst-intern</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>🧠 Szereted elemezni az összefüggéseket, és szívesen dolgoznál adatokkal üzleti környezetben? Akkor ez a pozíció remek lehetőség számodra. 🏢 Partnerünk a hazai távközlési piac teljes szolgáltatás-portfólióját elérhetővé teszi, legyen szó kommunikációs megoldásokról vagy szórakozásról. A cég tevékenysége révén három alapvető üzleti területet fed le: - vezetékes és mobilkommunikációs lakossági szolgáltatásokat - kis- és középvállalati szolgáltatásokat  - nagyvállalati ügyfeleknek nyújtott vállalati szolgáltatásokat. Főbb feladatok és felelősségek: 📊 Üzleti igények elemzése és támogatása 📊 Az igények megértése és azok megvalósulásának elősegítése 📊 Üzleti folyamatok E2E menedzselése 📊 Az üzleti kérdések összekötése a vállalat adatvagyonával 📊 Kimutatások és riportok készítése 📊 Adatbázisokon alapuló mély elemzések készítése 📊 Adatalapú válaszok kidolgozása üzleti-műszaki kérdésekre 📊 Üzleti döntéseket támogató vizualizációk elkészítése 📊 Javaslattétel a munkafolyamatok fejlesztésére 📊 Közreműködés technikai megoldások és ötletek kidolgozásában 📊 Aktív részvétel projektekben és specifikációk fejlesztésében 📊 Tesztelések kidolgozása és elvégzése 📊 Rendszeres tájékoztatás a vezetőség felé 📊 Szoros szakmai kapcsolattartás az üzleti területekkel 📊 Elemzések és riportok kommunikálása a stakeholderek felé Elvárások: 🐾 Folyamatban lévő felsőfokú tanulmány gazdaságtudományi, informatikai vagy távközléssel összefüggő szakon 🐾 Adatinfrastruktúrákban való alapfokú jártasság 🐾 SQL alapfokú felhasználói ismerete 🐾 Adatvizualizációs eszközök ismerete 🐾 Agilis módszertanok és eszközök ismerete 🐾 Középfokú angol nyelvtudás 🐾 Jó kommunikációs készségek 🐾 Analitikai gondolkodásmód és üzleti értékvezérelt szemlélet 🐾 Adatarchitektúra és adatmodellezés iránti érdeklődés 🐾 Üzleti érzék és az összefüggések feltérképezése 🐾 Rendszerszemlélet 🐾 Keresztfunkcionális csapatokkal való hatékony kommunikáció Munkakörnyezet: 🚀 Valódi szakmai fejlődés: Partnerünk legnagyobb adat platformjának építésében vehetsz részt 💡 Mentorálás: tapasztalt kollégáktól tanulhatod meg a modern szoftverfejlesztés és üzemeltetés alapjait 🕒 Rugalmasság: a tanulás az első, így a munkaidőt az egyetemi óráidhoz igazítják 🏠 Modern környezet: Home Office lehetőség és inspiráló irodai légkör ⏰ Munkaidő: A feladatokat és a munkaidőt a Partner osztja be, a tanulmányok figyelembevételével ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Középfokú angol nyelvtudás</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Budapest, IX. kerület + Home Office</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Br. 3000 Ft/óra*</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>ml_score=4, ml_prob=0.33623695194800135</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
+        <v>4</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.3362369519480014</v>
+      </c>
+      <c r="L40" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>schonherz</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Operation intern (Dataflow Monitoring and Deployment Squad)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40904-operation-intern-dataflow-monitoring-and-deployment-squad</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>💡 Szeretnél tapasztalt szakemberektől tanulni, miközben Partnerünk egyik legnagyobb adatplatformjának építésében vehetsz részt? Csatlakozz! 🏢 Partnerünk a hazai távközlési piac teljes szolgáltatás-portfólióját elérhetővé teszi, legyen szó kommunikációs megoldásokról vagy szórakozásról. A cég tevékenysége révén három alapvető üzleti területet fed le: - vezetékes és mobilkommunikációs lakossági szolgáltatásokat - kis- és középvállalati szolgáltatásokat  - nagyvállalati ügyfeleknek nyújtott vállalati szolgáltatásokat. Feladatok: 🔹 Aktív részvétel a squad mindennapi üzemeltetési feladataiban 🔹 A rendszerek monitorozása, elemzése, valamint javaslattétel a hibák elhárítására 🔹 Ismerkedés a felhőalapú infrastruktúrával, különösen a Google Cloud Platform (GCP) eszköztárával, és részvétel az üzemeltetési feladatokban Elvárások: 🟣 Folyamatban lévő felsőfokú szakirányú tanulmányok informatikai, mérnöki vagy matematikai területen 🟣 Alapszintű, magabiztos Python nyelvtudás 🟣 Az SQL alapelveinek ismerete, különös tekintettel a lekérdezésekre és a táblák kezelésére 🟣 Alapvető Linux/Unix parancssoros ismeretek, valamint a Git verziókezelő használata 🟣 Nyitottság az új technológiák gyors elsajátítására és proaktív hozzáállás Munkakörnyezet: 📈 Valódi szakmai fejlődési lehetőség, mivel a partner egyik legnagyobb adatplatformjának építésében lehet részt venni 🤝 Mentorálás tapasztalt kollégák által, akik segítenek elsajátítani a modern szoftverfejlesztés és üzemeltetés gyakorlati oldalát 🎓 Rugalmasság, hiszen a munkaidőt az egyetemi órarendhez igazítják 🏠 Home Office lehetőség és inspiráló irodai környezet ⏰ Munkaidő: A feladatokat és a munkaidőt a Partner osztja be, a tanulmányok figyelembevételével ❗ A jelentkezés menete: 1️⃣ Regisztráció a Schönherz.hu oldalon 2️⃣ Schönherz.hu oldalon  önéletrajz kitöltése *Amennyiben 25 éves elmúltál, a bruttó bérből 15% SZJA kerül levonásra. Ha 25 év alatt vagy, SZJA mentessé válsz, így a bruttó béredet nettóként tekintheted, a nemzetgazdasági átlagkereset mértékéig, ami 693 700 Ft havonta.</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Budapest, IX. kerület + Home Office</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Br. 3000 Ft/óra*</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>ml_score=4, ml_prob=0.3404202353236459</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
+        <v>4</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.3404202353236459</v>
+      </c>
+      <c r="L41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>muisz</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SOC Analyst gyakornok</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://muisz.hu/diakmunkaink/SOC%20Analyst%20gyakornok%20-budapest-i-kerulet--28367</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>SOC Analyst gyakornok Több mint 20 éve támogatjuk Ügyfeleinket, köztük jogszabályi megfelelés alá tartozó szervezeteket abban, hogy informatikai és információbiztonsági környezetük ne csak üzemeljen, hanem megfeleljen a hatályos szabályozásoknak és a NIS2 irányelv elvárásainak is. Most Téged is bevonnánk ebbe a munkába - valós biztonsági események kezelésébe, strukturált SOC folyamatok mentén, tapasztalt szakértők támogatásával. Feladatok Milyen feladatokra számíthatsz? - Naplóelemző és eseménykezelő rendszerekbe érkező biztonsági események első szintű (SOC Analyst L1) validálása - A jogszabály alá tartozó Ügyfelek biztonsági monitorozásának támogatása, a NIS2 elvárásoknak megfelelő működés elősegítése - Biztonsági riasztások elemzése, relevancia vizsgálata, false pozitív események azonosítása - Események státusz szerinti besorolása az incidenskezelő rendszerben (pl. lezárás false pozitív esetén, releváns események továbbítása magasabb szintre) - Események dokumentálása, alapvető elemzési megállapítások rögzítése - Részvétel ügyfeleknél történő biztonsági monitorozási megoldások bevezetésében, finomhangolásában - Riasztási zaj csökkentésének támogatása (use case-ek pontosítása, tapasztalatok visszacsatolása SOC szinten) Elvárások Téged keresünk, ha • Mérnök-informatikus, kiberbiztonsági mérnöki vagy hasonló informatikai szakon tanulsz nappali tagozaton • Érdeklődsz az információbiztonság és a kiberbiztonsági folyamatok iránt • Alapvető ismereteid vannak IT infrastruktúrákról (Windows rendszerek, hálózati alapok) • Pontos, szabálykövető szemlélettel dolgozol, és fontos számodra a dokumentáltság • Nem jelent problémát több esemény párhuzamos kezelése • Ügyfélorientált vagy, és jól működsz csapatban Előnyt jelent, ha • Van már tapasztalatod naplóelemzéssel vagy IT biztonsági területen • Találkoztál már vagy érdekelnek SIEM vagy logmenedzsment megoldások • El tudod képzelni nagyvonalakban az incidenskezelési folyamatokat • Érdekel a jogszabályi megfelelés (pl. NIS2, ISO 27001) gyakorlati oldala • Van hibajegykezelő vagy incidenskezelő rendszerrel szerzett tapasztalatod Egyéb Amit mi kínálunk • Valós környezetben szerezhető, piacképes kiberbiztonsági tapasztalat • Fokozatos betanulás, szakmai mentorálás • Szakmai kihívást jelentő, változatos feladatok • Együttműködő, támogató csapat • Színvonalas irodai munkakörnyezet • Családias, szakmailag elkötelezett légkör Szükséges nyelvtudás • Alapfokú angol nyelvtudás (dokumentációk, riasztások értelmezése) Munkavégzés helye • Budapest, Széll Kálmán tér</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Budapest 1. ker.</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2400 Ft/ óra</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>ml_score=3, ml_prob=0.2863907125094936</t>
+        </is>
+      </c>
+      <c r="J42" t="n">
+        <v>3</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.2863907125094936</v>
+      </c>
+      <c r="L42" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>muisz</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>IT Rendszerüzemeltető gyakornok</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://muisz.hu/diakmunkaink/IT%20Rendszer%C3%BCzemeltet%C5%91%20gyakornok--28368</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>IT Rendszerüzemeltető gyakornok Több mint 20 éve segítjük Ügyfeleinket abban, hogy az informatika ne csak működjön, hanem biztonságosan és hatékonyan szolgálja a napi üzletmenetet. Most Téged is bevonnánk ebbe – valós projekteken, segítőkész csapattársakkal. Feladatok Milyen feladatokra számíthatsz? •	Windows 11 számítógépek, valamint Windows alapú szerver infrastruktúra üzemeltetése, hibajavítása •	Hardver- és szoftver telepítése, adminisztrációja, hibaelhárítása •	Monitoring rendszerek követése, riasztások kezelése •	Központi vírusvédelmi rendszerek kezelése és üzemeltetése •	Biztonsági mentések ellenőrzése és üzemeltetése •	M365 szolgáltatások (Outlook, SharePoint, OneDrive, stb.) üzemeltetése és kezelése •	Felhasználók támogatása - távolról, vagy akár helyszínen •	IT problémák gyors, önálló megoldása Elvárások Téged keresünk, ha •	Mérnök-informatikus vagy hasonló szakon tanulsz nappali tagozaton •	Képben vagy Windows 11 rendszerekkel és irodai alkalmazásokkal (Office, Outlook, Teams, stb.) •	Nem ijedsz meg attól, ha két dolgot is kell csinálni egyszerre •	Ügyfélorientált vagy és szívesen dolgozol csapatban is •	Képes vagy a felmerülő problémák kezelésére és törekszel a gyors megoldásra •	Alapfokú angol nyelvtudás Előnyt jelent, ha •	Van már releváns szakmai tapasztalatod •	Dolgoztál már hibajegykezelő rendszerekkel •	Rendelkezel már központilag menedzselt vírusvédelmi rendszerek használatában szerzett tapasztalattal •	Láttál már, esetleg dolgoztál is monitoring rendszerekkel •	Ismered az M365 legalapvetőbb szolgáltatásait, mint pl. SharePoint, OneDrive, Outlook •	Találkoztál már biztonsági mentésre használt rendszerekkel Egyéb Amit mi kínálunk: •	Értékes és hasznos szakmai tapasztalat •	Szakmai kihívást jelentő, változatos feladatok •	Fiatalos, lendületes, együttműködő csapat •	Színvonalas irodai munkakörnyezet •	Családias légkör Szükséges nyelvtudás: Munkavégzés helye: •	Budapest, Széll Kálmán tér</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Budapest 1. ker.</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2400 Ft/ óra</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>ml_score=3, ml_prob=0.2917274156294231</t>
+        </is>
+      </c>
+      <c r="J43" t="n">
+        <v>3</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.2917274156294231</v>
+      </c>
+      <c r="L43" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Migrate job labeling and storage to database
Refactored job labeling endpoint in app.py to use the database for storing labels instead of file-based storage, with validation for label values. Updated main.py to save job data directly to the database, removing interactive labeling and file-based label persistence. Also updated seen jobs lists and job data export.
</commit_message>
<xml_diff>
--- a/data/jobs.xlsx
+++ b/data/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,11 @@
           <t>ml_score</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>job_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -538,6 +543,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -582,6 +588,7 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -622,6 +629,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -666,6 +674,7 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -706,6 +715,7 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -750,6 +760,7 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -794,6 +805,7 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -838,6 +850,7 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -882,6 +895,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -896,6 +910,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -944,6 +959,7 @@
       <c r="L12" t="n">
         <v>5</v>
       </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -996,6 +1012,7 @@
       <c r="L13" t="n">
         <v>5</v>
       </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1048,6 +1065,7 @@
       <c r="L14" t="n">
         <v>4</v>
       </c>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1100,6 +1118,7 @@
       <c r="L15" t="n">
         <v>5</v>
       </c>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1152,6 +1171,7 @@
       <c r="L16" t="n">
         <v>4</v>
       </c>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1204,6 +1224,7 @@
       <c r="L17" t="n">
         <v>3</v>
       </c>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1256,6 +1277,7 @@
       <c r="L18" t="n">
         <v>5</v>
       </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1308,6 +1330,7 @@
       <c r="L19" t="n">
         <v>3</v>
       </c>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1360,6 +1383,7 @@
       <c r="L20" t="n">
         <v>3</v>
       </c>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1412,6 +1436,7 @@
       <c r="L21" t="n">
         <v>3</v>
       </c>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1464,6 +1489,7 @@
       <c r="L22" t="n">
         <v>3</v>
       </c>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1516,6 +1542,7 @@
       <c r="L23" t="n">
         <v>3</v>
       </c>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1568,6 +1595,7 @@
       <c r="L24" t="n">
         <v>3</v>
       </c>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1622,6 +1650,7 @@
       <c r="L25" t="n">
         <v>4</v>
       </c>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1676,6 +1705,7 @@
       <c r="L26" t="n">
         <v>3</v>
       </c>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1726,6 +1756,7 @@
       <c r="L27" t="n">
         <v>3</v>
       </c>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1780,6 +1811,7 @@
       <c r="L28" t="n">
         <v>4</v>
       </c>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1830,6 +1862,7 @@
       <c r="L29" t="n">
         <v>3</v>
       </c>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1880,6 +1913,7 @@
       <c r="L30" t="n">
         <v>5</v>
       </c>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1934,6 +1968,7 @@
       <c r="L31" t="n">
         <v>3</v>
       </c>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1988,6 +2023,7 @@
       <c r="L32" t="n">
         <v>3</v>
       </c>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2042,6 +2078,7 @@
       <c r="L33" t="n">
         <v>4</v>
       </c>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2096,6 +2133,7 @@
       <c r="L34" t="n">
         <v>3</v>
       </c>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2150,6 +2188,7 @@
       <c r="L35" t="n">
         <v>3</v>
       </c>
+      <c r="M35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2204,6 +2243,7 @@
       <c r="L36" t="n">
         <v>4</v>
       </c>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2258,6 +2298,7 @@
       <c r="L37" t="n">
         <v>3</v>
       </c>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2312,6 +2353,7 @@
       <c r="L38" t="n">
         <v>3</v>
       </c>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2362,6 +2404,7 @@
       <c r="L39" t="n">
         <v>4</v>
       </c>
+      <c r="M39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2416,6 +2459,7 @@
       <c r="L40" t="n">
         <v>4</v>
       </c>
+      <c r="M40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2466,6 +2510,7 @@
       <c r="L41" t="n">
         <v>4</v>
       </c>
+      <c r="M41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2516,6 +2561,7 @@
       <c r="L42" t="n">
         <v>3</v>
       </c>
+      <c r="M42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2566,6 +2612,7 @@
       <c r="L43" t="n">
         <v>3</v>
       </c>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2620,6 +2667,7 @@
       <c r="L44" t="n">
         <v>3</v>
       </c>
+      <c r="M44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2673,6 +2721,172 @@
       </c>
       <c r="L45" t="n">
         <v>4</v>
+      </c>
+      <c r="M45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>schonherz</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Web Developer Intern - Calibration Team</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://schonherz.hu/diakmunka/budapest/fejleszto---tesztelo/40918-web-developer-intern-calibration-team</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>🔐 Work on real autonomous driving projects as a Web Developer Intern in a friendly, small team. You’ll build data-driven web applications for sensor calibration and analytics while gaining hands-on experience in automotive R&amp;D with flexible hours and long-term opportunities. 🚗 Our Partner is a software development company specializing in autonomous vehicles. Their primary approach to self-driving technology is camera-based, relying on image processing, while also experimenting with radar and lidar solutions. The company is Hungarian-owned, yet operates with a distinctly American-style, relaxed management culture, works on numerous U.S.-based projects, and offers internal career advancement opportunities. 🪂 Developing automated driving requires a complete and mature toolchain to collect, generate, use, and manage the data needed for a safe and robust solution. A modern, data-driven pipeline for automated driving reduces the complexity of data processing through a high level of automation, while still ensuring automotive-grade quality. Sensors are the most important link between the system and its environment. Precise sensor calibration and a deep understanding of how sensors perceive the world are essential for self-driving applications. As a web developer intern in a small team, the intern takes part in the development of calibration and diagnostic data analytics pipelines and supports the team’s daily work through coding and testing. Job Summary 🌀 Collaborating closely with research colleagues to create visualizations for cutting-edge sensor calibration algorithms (React.js, Python) 🌀 Contribute to the development and testing of the calibration and diagnostic pipeline by building intuitive web applications to enhance data comprehension (JavaScript, Python) 🌀 Collaborate with users and the design team to enhance the user experience 🌀 Ensure the functionality and upkeep of the calibration and diagnostic database through thorough testing and maintenance (SQL) 🌀 Assist the team in developing and maintaining an automated testing pipeline, as well as supporting manual testing efforts Expectations: 🟨 Ongoing (active/passive) full-time university studies for at least one more year 🟨 Solid Python and React.js knowledge 🟨 Intermediate level English knowledge 🟨 Availability of at least 20 working hours per week 🟨 Ability to work independently What our Partner offers: 📍 Possibility to gain valuable work experience at the forefront of the automotive R&amp;D sector 💸 Competitive student salary 💡 Inspiring and supportive working environment 🎳 Teambuilding events and other benefits for students ⏳ Flexible working hours 📗 Long-term job opportunity 🫟 Possibility of an immediate start 🧷 In-service training opportunity 🏋️ Fitness opportunities 🥯 Free lunch every workday at one of the best all-you-can-eat restaurants in Budapest or delivered by Wolt for Work ⏰ Working hours: From 8:00 a.m. to 6:00 p.m. ❗ How to apply: 1️⃣ Register on Schönherz.hu 2️⃣ Fill in a CV on Schönherz.hu * If you are over 25 years of age, 15% of your gross salary will be deducted from your PIT. If you are under 25 years old, you will be exempt from PIT, so you can consider your gross salary as net, up to the average wage in the national economy, which is HUF 693,700 per month.</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>English (Intermediate)</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Budapest, District II. + Home Office</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Gross 2250-2500 Ft/hour*</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>ml_score=3, ml_prob=0.28012610847425057</t>
+        </is>
+      </c>
+      <c r="J46" t="n">
+        <v>3</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.2801261084742506</v>
+      </c>
+      <c r="L46" t="n">
+        <v>3</v>
+      </c>
+      <c r="M46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>muisz</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Test Engineer (Intern) on Industrial Automation Field</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://muisz.hu/diakmunkaink/test-engineer-%20Industrial-Automation-Field-trainee-xi-kerulet--28375</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Test Engineer (Intern) on Industrial Automation Field Today the community of around 1800 IT professionals and engineers believe - along with me - that the evosoft team is the place for us. Our co-workers in Budapest, Miskolc and Szeged are busy writing software which, although invisible to the naked eye, can fundamentally influence the very basics of our everyday lives. You will come across our software solutions in different kinds of the largest medical equipment technology, not to mention that our codes drive the greatest car manufacturers’ automation systems and you can even find them/us in electric cars. There are hardly any industrial areas where the programs I and my colleagues tested or developed are not present. The company evosoft, in its full name evosoft Hungary Kft. (Ltd.) started with 3 members more than 30 years ago. As of today, our headcount has reached the 1800 employees and we are expanding - join us, be part of our team!" Would you like to get to know those Siemens devices, which control the world’s largest and most innovative factories? Would you like to be part of a professional team, where you can constantly challenge yourself in your daily work? Would you like to work in an attractive lab environment, where you can constantly develop yourself as part of a dynamic team? If your answer is YES, then read our offer below! Feladatok •	Working closely with Test Engineers and Developers to understand product requirements and ensure high quality in releases •	Testing Siemens SIMATIC S7 PLC and HMI product families’ engineering systems and hardwares •	Executing test cases (manual and/or automated) and analyzing results •	Writing and maintaining test plans / test cases •	Designing and building hardware configurations for tests •	Bug analysis, documentation and follow up in the bug documenting system •	Participation in the setup of the test environment Elvárások •	Ongoing higher education (electrical engineer, software engineer, mechanical engineer, mechatronics engineer or similar) •	Basic electrical knowledge •	Knowledge of MS Windows 11, MS Office •	Communication level English language skills •	Ability to work independently and in a team, flexibility •	Independent, able to solve problems, analytical mindset •	Motivation to continuous self-development Egyéb Advantages: •	PLC programming knowledge (e.g. STL / SCL / FBD / LAD) •	Knowledge of Siemens SIMATIC S7-300 / 400 / 1200 / 1500 PLC product families •	Knowledge of Siemens STEP7 / TIA Portal product families •	C# and/or Python programming knowledge What we offer: •	Real-world experience in agile development processes •	You can work on various challenging tasks in the field of industrial automation •	Flexible working hours and the option to work remotely •	A dynamic, supporting team with mentor(s) •	Attractive working environment and secure workplace •	Free coffee and fruit days •	Recreational opportunities within the office building (table tennis, darts etc.) •	Various career opportunities •	Joining possibility to our different communities: sports communities, CSR, green, ToastMasters etc. •	Parking lot within the office building</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>magyar, angol</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Budapest 11. ker.</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2200-2800 Ft/óra</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>ml_score=3, ml_prob=0.2318041591459815</t>
+        </is>
+      </c>
+      <c r="J47" t="n">
+        <v>3</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.2318041591459815</v>
+      </c>
+      <c r="L47" t="n">
+        <v>3</v>
+      </c>
+      <c r="M47" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>muisz</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Android developer trainee</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://muisz.hu/diakmunkaink/Android-developer-trainee-III-kerulet--27760</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Android developer trainee Android developer trainee Feladatok The main task of the candidate would be to write unit tests for already completed components, for which it would be useful to use AI assistance. What would be your responsibilities? •	Develop HMI components for automotive cockpit systems •	Implement unit tests and other improvements for components •	Support integration with vehicle middleware and hardware on Android Automotive OS Elvárások The ideal candidate should possess experience in the following •	Kotlin development •	Android HMI •	MVVM pattern and unit testing •	AI assistance in software development •	MS Teams, Jira, Confluence and Bitbucket/Git •	Good verbal and written English Egyéb - Participate in team meetings and brainstorming sessions, contributing ideas for new marketing campaigns and content strategies. - Assist with the creation of marketing materials, including brochures, flyers, and presentations, as needed. - Perform administrative tasks related to marketing projects and campaigns, ensuring smooth operations within the team.</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>magyar, angol</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Budapest 3. ker.</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2600 Ft/óra</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>ml_score=3, ml_prob=0.2557808943824647</t>
+        </is>
+      </c>
+      <c r="J48" t="n">
+        <v>3</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.2557808943824647</v>
+      </c>
+      <c r="L48" t="n">
+        <v>3</v>
+      </c>
+      <c r="M48" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>